<commit_message>
Add pagination; change image URL property to dropbox file path
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E878C9-2F78-4E34-99AF-476077E95E47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71622872-BE11-4E2B-885B-0DADB5004434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -216,16 +216,31 @@
     <t>Tag5</t>
   </si>
   <si>
-    <t>Image URL</t>
-  </si>
-  <si>
-    <t>https://www.dropbox.com/scl/fi/akoxjrznd147egjombm2y/DyeSubHoodie-SEIU-Pattern1_2000px.jpg?rlkey=xp1wmkbtj0porep070j34vt89&amp;dl=0</t>
-  </si>
-  <si>
-    <t>https://www.dropbox.com/scl/fi/k8cdvdncoamt1qqj49lzr/DyeSubHoodie-SEIU-Pattern2_2000px.jpg?rlkey=y82zqdqkkbsayp24nyh3dtoty&amp;dl=0</t>
-  </si>
-  <si>
-    <t>https://www.dropbox.com/scl/fi/rtqt92cpanyiyi3w2o4j7/DyeSubHoodie-SEIU-Pattern3_2000px.jpg?rlkey=23dhls1v3f9je5i2m66knhzau&amp;dl=0</t>
+    <t>Dropbox Image Path</t>
+  </si>
+  <si>
+    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1645.jpg</t>
+  </si>
+  <si>
+    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1646.jpg</t>
+  </si>
+  <si>
+    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1647.jpg</t>
+  </si>
+  <si>
+    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1648.jpg</t>
+  </si>
+  <si>
+    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1649.jpg</t>
+  </si>
+  <si>
+    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1650.jpg</t>
+  </si>
+  <si>
+    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1651.jpg</t>
+  </si>
+  <si>
+    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1652.jpg</t>
   </si>
 </sst>
 </file>
@@ -579,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +775,7 @@
         <v>49</v>
       </c>
       <c r="P5" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -786,7 +801,7 @@
         <v>47</v>
       </c>
       <c r="P6" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -818,7 +833,7 @@
         <v>46</v>
       </c>
       <c r="P7" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -844,7 +859,7 @@
         <v>50</v>
       </c>
       <c r="P8" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -873,7 +888,7 @@
         <v>50</v>
       </c>
       <c r="P9" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add non-blocking requests for Dropbox file URLs; make endpoints only get URLs for the designs that are not excluded by filters, pagination, etc.; remove lazy loading of temp db file
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71622872-BE11-4E2B-885B-0DADB5004434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB7E77C-CE62-4882-AD33-1795CF952975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -594,8 +594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
   <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add ID to temp design data; add support for getting a single design by ID
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB7E77C-CE62-4882-AD33-1795CF952975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4623E2DB-DBA9-4B10-88C5-0FA2C0A40F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1652.jpg</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -592,314 +595,341 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="90.140625" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="16" max="16" width="131.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="90.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="17" max="17" width="131.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>51</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>52</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>53</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>54</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>55</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1025</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>36</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>41</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>40</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
       </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
       <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
         <v>49</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1009</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>48</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1006</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>35</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>40</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>43</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>19</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>47</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1003</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>37</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>19</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>46</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>47</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>49</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>44</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>20</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>19</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>47</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>45</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>42</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>20</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>19</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>47</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>46</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>38</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>41</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>19</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>20</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>50</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1001</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>34</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>36</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>40</v>
-      </c>
-      <c r="I9" t="s">
-        <v>19</v>
       </c>
       <c r="J9" t="s">
         <v>19</v>
       </c>
       <c r="K9" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" t="s">
         <v>50</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>64</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:J1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:K1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:H1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:I1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
       <formula1>Subcategories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:O1048576" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:P1048576" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
       <formula1>Tags</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Update data model for temp db
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4623E2DB-DBA9-4B10-88C5-0FA2C0A40F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F723F-2A9F-4130-955A-91385D4B5910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Designs" sheetId="1" r:id="rId1"/>
-    <sheet name="Tags" sheetId="5" r:id="rId2"/>
-    <sheet name="Categories" sheetId="2" r:id="rId3"/>
-    <sheet name="Subcategories" sheetId="3" r:id="rId4"/>
-    <sheet name="YesNo" sheetId="4" r:id="rId5"/>
+    <sheet name="DesignType" sheetId="6" r:id="rId2"/>
+    <sheet name="Tags" sheetId="5" r:id="rId3"/>
+    <sheet name="Categories" sheetId="2" r:id="rId4"/>
+    <sheet name="Subcategories" sheetId="3" r:id="rId5"/>
+    <sheet name="YesNo" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Categories">Categories!$A$2:$A$1048576</definedName>
+    <definedName name="DesignType">DesignType!$A$1:$A$2</definedName>
     <definedName name="Subcategories">Subcategories!$C$2:$C$1048576</definedName>
     <definedName name="Tags">Tags!$A$2:$A$1048576</definedName>
     <definedName name="YesNo">YesNo!$A$1:$A$2</definedName>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="122">
   <si>
     <t>Name</t>
   </si>
@@ -60,12 +62,6 @@
     <t>Holiday</t>
   </si>
   <si>
-    <t>Strikes</t>
-  </si>
-  <si>
-    <t>Negotiations</t>
-  </si>
-  <si>
     <t>Eagle</t>
   </si>
   <si>
@@ -78,9 +74,6 @@
     <t>Parent Category</t>
   </si>
   <si>
-    <t>Christmas</t>
-  </si>
-  <si>
     <t>Labor Day</t>
   </si>
   <si>
@@ -111,24 +104,9 @@
     <t>No</t>
   </si>
   <si>
-    <t>Union-Specific</t>
-  </si>
-  <si>
-    <t>Big Strike</t>
-  </si>
-  <si>
-    <t>Little Strike</t>
-  </si>
-  <si>
-    <t>Wages</t>
-  </si>
-  <si>
     <t>SEIU</t>
   </si>
   <si>
-    <t>IBEW</t>
-  </si>
-  <si>
     <t>IUPAT</t>
   </si>
   <si>
@@ -168,24 +146,6 @@
     <t>Hierarchy</t>
   </si>
   <si>
-    <t>Strikes &gt; Big Strike</t>
-  </si>
-  <si>
-    <t>Holiday &gt; Christmas</t>
-  </si>
-  <si>
-    <t>Negotiations &gt; Wages</t>
-  </si>
-  <si>
-    <t>Union-Specific &gt; SEIU</t>
-  </si>
-  <si>
-    <t>Union-Specific &gt; IUPAT</t>
-  </si>
-  <si>
-    <t>Holiday &gt; Labor Day</t>
-  </si>
-  <si>
     <t>Patriotic</t>
   </si>
   <si>
@@ -216,9 +176,6 @@
     <t>Tag5</t>
   </si>
   <si>
-    <t>Dropbox Image Path</t>
-  </si>
-  <si>
     <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1645.jpg</t>
   </si>
   <si>
@@ -243,7 +200,220 @@
     <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1652.jpg</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>Design Type</t>
+  </si>
+  <si>
+    <t>Quick Search</t>
+  </si>
+  <si>
+    <t>Event/Awareness</t>
+  </si>
+  <si>
+    <t>Union Specific</t>
+  </si>
+  <si>
+    <t>Location Specific</t>
+  </si>
+  <si>
+    <t>Featured</t>
+  </si>
+  <si>
+    <t>New Designs</t>
+  </si>
+  <si>
+    <t>Best Sellers</t>
+  </si>
+  <si>
+    <t>Staff Favorites</t>
+  </si>
+  <si>
+    <t>Classics</t>
+  </si>
+  <si>
+    <t>Economy</t>
+  </si>
+  <si>
+    <t>Ladies</t>
+  </si>
+  <si>
+    <t>Strike &amp; Negotiations</t>
+  </si>
+  <si>
+    <t>Golf</t>
+  </si>
+  <si>
+    <t>Picnics</t>
+  </si>
+  <si>
+    <t>Anniversary</t>
+  </si>
+  <si>
+    <t>Political</t>
+  </si>
+  <si>
+    <t>Breast Cancer</t>
+  </si>
+  <si>
+    <t>St. Patrick's Day</t>
+  </si>
+  <si>
+    <t>Veterans Day</t>
+  </si>
+  <si>
+    <t>International Logos</t>
+  </si>
+  <si>
+    <t>APWU</t>
+  </si>
+  <si>
+    <t>BAC</t>
+  </si>
+  <si>
+    <t>Boilermakers</t>
+  </si>
+  <si>
+    <t>Carpenters</t>
+  </si>
+  <si>
+    <t>CWA</t>
+  </si>
+  <si>
+    <t>Electrical Workers</t>
+  </si>
+  <si>
+    <t>IAFF</t>
+  </si>
+  <si>
+    <t>IAM</t>
+  </si>
+  <si>
+    <t>IATSE</t>
+  </si>
+  <si>
+    <t>Ironworkers</t>
+  </si>
+  <si>
+    <t>Heat &amp; Frost Insulators</t>
+  </si>
+  <si>
+    <t>IUEC</t>
+  </si>
+  <si>
+    <t>IUOE</t>
+  </si>
+  <si>
+    <t>Laborers</t>
+  </si>
+  <si>
+    <t>Mailhandlers</t>
+  </si>
+  <si>
+    <t>NATCA</t>
+  </si>
+  <si>
+    <t>NALC</t>
+  </si>
+  <si>
+    <t>NEA</t>
+  </si>
+  <si>
+    <t>OPCMIA</t>
+  </si>
+  <si>
+    <t>OPEIU</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Nurses</t>
+  </si>
+  <si>
+    <t>Roofers</t>
+  </si>
+  <si>
+    <t>SMART</t>
+  </si>
+  <si>
+    <t>Teamsters</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>UAW</t>
+  </si>
+  <si>
+    <t>UWUA</t>
+  </si>
+  <si>
+    <t>USW</t>
+  </si>
+  <si>
+    <t>Sleeve</t>
+  </si>
+  <si>
+    <t>Oversize</t>
+  </si>
+  <si>
+    <t>Youth/Kids</t>
+  </si>
+  <si>
+    <t>Holiday &gt; Veterans Day</t>
+  </si>
+  <si>
+    <t>Quick Search &gt; Featured</t>
+  </si>
+  <si>
+    <t>Quick Search &gt; New Designs</t>
+  </si>
+  <si>
+    <t>Event/Awareness &gt; Golf</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; IAM</t>
+  </si>
+  <si>
+    <t>Location Specific &gt; Oversize</t>
+  </si>
+  <si>
+    <t>Quick Search &gt; Classics</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; International Logos</t>
+  </si>
+  <si>
+    <t>Quick Search &gt; Staff Favorites</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; NALC</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; SEIU</t>
+  </si>
+  <si>
+    <t>Design Number</t>
+  </si>
+  <si>
+    <t>Dropbox Image Path 1</t>
+  </si>
+  <si>
+    <t>Dropbox Image Path 3</t>
+  </si>
+  <si>
+    <t>Dropbox Image Path 2</t>
+  </si>
+  <si>
+    <t>Dropbox Image Path 4</t>
+  </si>
+  <si>
+    <t>Dropbox Image Path 5</t>
+  </si>
+  <si>
+    <t>Dropbox Image Path 6</t>
+  </si>
+  <si>
+    <t>This sheet should not be edited.</t>
   </si>
 </sst>
 </file>
@@ -595,26 +765,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="90.140625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5703125" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="17" max="17" width="131.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="17" max="17" width="71.85546875" customWidth="1"/>
+    <col min="18" max="18" width="63.85546875" customWidth="1"/>
+    <col min="19" max="19" width="59.42578125" customWidth="1"/>
+    <col min="20" max="20" width="60.140625" customWidth="1"/>
+    <col min="21" max="21" width="61.42578125" customWidth="1"/>
+    <col min="22" max="22" width="57.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -626,311 +804,359 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>17</v>
-      </c>
       <c r="K1" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="M1" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="N1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="O1" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="P1" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="Q1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="R1" t="s">
+        <v>117</v>
+      </c>
+      <c r="S1" t="s">
+        <v>116</v>
+      </c>
+      <c r="T1" t="s">
+        <v>118</v>
+      </c>
+      <c r="U1" t="s">
+        <v>119</v>
+      </c>
+      <c r="V1" t="s">
+        <v>120</v>
+      </c>
+      <c r="W1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1025</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" t="s">
-        <v>19</v>
+        <v>103</v>
+      </c>
+      <c r="G2" t="s">
+        <v>104</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L2" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="Q2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="R2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1009</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" t="s">
+        <v>15</v>
+      </c>
+      <c r="L3" t="s">
         <v>34</v>
       </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" t="s">
-        <v>20</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="Q3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" t="s">
+        <v>44</v>
+      </c>
+      <c r="S3" t="s">
         <v>48</v>
       </c>
-      <c r="Q3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1006</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J4" t="s">
-        <v>20</v>
+        <v>109</v>
+      </c>
+      <c r="H4" t="s">
+        <v>113</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="Q4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1003</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>106</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>32</v>
+      </c>
+      <c r="M5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" t="s">
-        <v>47</v>
-      </c>
       <c r="N5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="Q5" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" t="s">
         <v>44</v>
       </c>
-      <c r="J6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K6" t="s">
-        <v>19</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="S6" t="s">
+        <v>43</v>
+      </c>
+      <c r="T6" t="s">
+        <v>48</v>
+      </c>
+      <c r="U6" t="s">
         <v>47</v>
       </c>
-      <c r="Q6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="V6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>42</v>
-      </c>
-      <c r="J7" t="s">
-        <v>20</v>
+        <v>108</v>
+      </c>
+      <c r="G7" t="s">
+        <v>111</v>
       </c>
       <c r="K7" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q7" t="s">
         <v>47</v>
       </c>
-      <c r="M7" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>109</v>
       </c>
       <c r="K8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="Q8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="R8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1001</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G9" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
         <v>36</v>
       </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" t="s">
-        <v>40</v>
-      </c>
-      <c r="J9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" t="s">
-        <v>50</v>
-      </c>
       <c r="Q9" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:K1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:I1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:J1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
       <formula1>Subcategories</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:P1048576" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
       <formula1>Tags</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{D0466454-C892-488E-AA3C-A206F5B6F670}">
+      <formula1>DesignType</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -939,6 +1165,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A83CC9-1574-4180-85AD-01F92A9D1604}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096F644A-6816-46A6-9C37-F543D22E3BF1}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -955,27 +1211,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -983,12 +1239,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE8B92B-2F2F-44F6-BB2D-490F7DE9352F}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,22 +1259,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1027,17 +1288,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1586536D-3214-4B71-B711-EFBAF2410143}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.140625" customWidth="1"/>
   </cols>
@@ -1047,111 +1308,627 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C2" t="str">
         <f>_xlfn.CONCAT(B2, " &gt; ", A2)</f>
-        <v>Holiday &gt; Christmas</v>
+        <v>Quick Search &gt; New Designs</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C9" si="0">_xlfn.CONCAT(B3, " &gt; ", A3)</f>
-        <v>Holiday &gt; Labor Day</v>
+        <f>_xlfn.CONCAT(B3, " &gt; ", A3)</f>
+        <v>Quick Search &gt; Best Sellers</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C4" t="str">
-        <f t="shared" si="0"/>
-        <v>Strikes &gt; Big Strike</v>
+        <f>_xlfn.CONCAT(B4, " &gt; ", A4)</f>
+        <v>Quick Search &gt; Staff Favorites</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v>Strikes &gt; Little Strike</v>
+        <f>_xlfn.CONCAT(B5, " &gt; ", A5)</f>
+        <v>Quick Search &gt; Classics</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>51</v>
       </c>
       <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v>Negotiations &gt; Wages</v>
+        <f>_xlfn.CONCAT(B6, " &gt; ", A6)</f>
+        <v>Quick Search &gt; Patriotic</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v>Union-Specific &gt; SEIU</v>
+        <f>_xlfn.CONCAT(B7, " &gt; ", A7)</f>
+        <v>Quick Search &gt; Economy</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v>Union-Specific &gt; IBEW</v>
+        <f>_xlfn.CONCAT(B8, " &gt; ", A8)</f>
+        <v>Quick Search &gt; Ladies</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>52</v>
       </c>
       <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v>Union-Specific &gt; IUPAT</v>
+        <f>_xlfn.CONCAT(B9, " &gt; ", A9)</f>
+        <v>Event/Awareness &gt; Strike &amp; Negotiations</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="str">
+        <f>_xlfn.CONCAT(B10, " &gt; ", A10)</f>
+        <v>Event/Awareness &gt; Golf</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" t="str">
+        <f>_xlfn.CONCAT(B11, " &gt; ", A11)</f>
+        <v>Event/Awareness &gt; Picnics</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="str">
+        <f>_xlfn.CONCAT(B12, " &gt; ", A12)</f>
+        <v>Event/Awareness &gt; Anniversary</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" t="str">
+        <f>_xlfn.CONCAT(B13, " &gt; ", A13)</f>
+        <v>Event/Awareness &gt; Political</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="str">
+        <f>_xlfn.CONCAT(B14, " &gt; ", A14)</f>
+        <v>Event/Awareness &gt; Breast Cancer</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="str">
+        <f>_xlfn.CONCAT(B15, " &gt; ", A15)</f>
+        <v>Holiday &gt; Labor Day</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="str">
+        <f>_xlfn.CONCAT(B16, " &gt; ", A16)</f>
+        <v>Holiday &gt; St. Patrick's Day</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3</v>
+      </c>
+      <c r="C17" t="str">
+        <f>_xlfn.CONCAT(B17, " &gt; ", A17)</f>
+        <v>Holiday &gt; Veterans Day</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="str">
+        <f>_xlfn.CONCAT(B18, " &gt; ", A18)</f>
+        <v>Union Specific &gt; International Logos</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="str">
+        <f>_xlfn.CONCAT(B19, " &gt; ", A19)</f>
+        <v>Union Specific &gt; APWU</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C20" t="str">
+        <f>_xlfn.CONCAT(B20, " &gt; ", A20)</f>
+        <v>Union Specific &gt; BAC</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="str">
+        <f>_xlfn.CONCAT(B21, " &gt; ", A21)</f>
+        <v>Union Specific &gt; Boilermakers</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>74</v>
+      </c>
+      <c r="B22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" t="str">
+        <f>_xlfn.CONCAT(B22, " &gt; ", A22)</f>
+        <v>Union Specific &gt; Carpenters</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="str">
+        <f>_xlfn.CONCAT(B23, " &gt; ", A23)</f>
+        <v>Union Specific &gt; CWA</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" t="str">
+        <f>_xlfn.CONCAT(B24, " &gt; ", A24)</f>
+        <v>Union Specific &gt; Electrical Workers</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" t="str">
+        <f>_xlfn.CONCAT(B25, " &gt; ", A25)</f>
+        <v>Union Specific &gt; IAFF</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="str">
+        <f>_xlfn.CONCAT(B26, " &gt; ", A26)</f>
+        <v>Union Specific &gt; IAM</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" t="str">
+        <f>_xlfn.CONCAT(B27, " &gt; ", A27)</f>
+        <v>Union Specific &gt; IATSE</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" t="str">
+        <f>_xlfn.CONCAT(B28, " &gt; ", A28)</f>
+        <v>Union Specific &gt; Ironworkers</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" t="str">
+        <f>_xlfn.CONCAT(B29, " &gt; ", A29)</f>
+        <v>Union Specific &gt; Heat &amp; Frost Insulators</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="str">
+        <f>_xlfn.CONCAT(B30, " &gt; ", A30)</f>
+        <v>Union Specific &gt; IUEC</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" t="str">
+        <f>_xlfn.CONCAT(B31, " &gt; ", A31)</f>
+        <v>Union Specific &gt; IUOE</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" t="str">
+        <f>_xlfn.CONCAT(B32, " &gt; ", A32)</f>
+        <v>Union Specific &gt; IUPAT</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" t="str">
+        <f>_xlfn.CONCAT(B33, " &gt; ", A33)</f>
+        <v>Union Specific &gt; Laborers</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>85</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" t="str">
+        <f>_xlfn.CONCAT(B34, " &gt; ", A34)</f>
+        <v>Union Specific &gt; Mailhandlers</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>86</v>
+      </c>
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="C35" t="str">
+        <f>_xlfn.CONCAT(B35, " &gt; ", A35)</f>
+        <v>Union Specific &gt; NATCA</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" t="str">
+        <f>_xlfn.CONCAT(B36, " &gt; ", A36)</f>
+        <v>Union Specific &gt; NALC</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>88</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="str">
+        <f>_xlfn.CONCAT(B37, " &gt; ", A37)</f>
+        <v>Union Specific &gt; NEA</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="str">
+        <f>_xlfn.CONCAT(B38, " &gt; ", A38)</f>
+        <v>Union Specific &gt; OPCMIA</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>90</v>
+      </c>
+      <c r="B39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C39" t="str">
+        <f>_xlfn.CONCAT(B39, " &gt; ", A39)</f>
+        <v>Union Specific &gt; OPEIU</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" t="str">
+        <f>_xlfn.CONCAT(B40, " &gt; ", A40)</f>
+        <v>Union Specific &gt; PASS</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" t="str">
+        <f>_xlfn.CONCAT(B41, " &gt; ", A41)</f>
+        <v>Union Specific &gt; Nurses</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" t="str">
+        <f>_xlfn.CONCAT(B42, " &gt; ", A42)</f>
+        <v>Union Specific &gt; Roofers</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C43" t="str">
+        <f>_xlfn.CONCAT(B43, " &gt; ", A43)</f>
+        <v>Union Specific &gt; SEIU</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" t="str">
+        <f>_xlfn.CONCAT(B44, " &gt; ", A44)</f>
+        <v>Union Specific &gt; SMART</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>95</v>
+      </c>
+      <c r="B45" t="s">
+        <v>53</v>
+      </c>
+      <c r="C45" t="str">
+        <f>_xlfn.CONCAT(B45, " &gt; ", A45)</f>
+        <v>Union Specific &gt; Teamsters</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" t="str">
+        <f>_xlfn.CONCAT(B46, " &gt; ", A46)</f>
+        <v>Union Specific &gt; UA</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" t="str">
+        <f>_xlfn.CONCAT(B47, " &gt; ", A47)</f>
+        <v>Union Specific &gt; UAW</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>98</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" t="str">
+        <f>_xlfn.CONCAT(B48, " &gt; ", A48)</f>
+        <v>Union Specific &gt; UWUA</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" t="str">
+        <f>_xlfn.CONCAT(B49, " &gt; ", A49)</f>
+        <v>Union Specific &gt; USW</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>100</v>
+      </c>
+      <c r="B50" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" t="str">
+        <f>_xlfn.CONCAT(B50, " &gt; ", A50)</f>
+        <v>Location Specific &gt; Sleeve</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" t="str">
+        <f>_xlfn.CONCAT(B51, " &gt; ", A51)</f>
+        <v>Location Specific &gt; Oversize</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" t="s">
+        <v>54</v>
+      </c>
+      <c r="C52" t="str">
+        <f>_xlfn.CONCAT(B52, " &gt; ", A52)</f>
+        <v>Location Specific &gt; Youth/Kids</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{2E446173-9549-4294-9E21-30D2EFE6849D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B1048576 B2:B52" xr:uid="{2E446173-9549-4294-9E21-30D2EFE6849D}">
       <formula1>Categories</formula1>
     </dataValidation>
   </dataValidations>
@@ -1159,24 +1936,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBDC08E-FD24-497A-86A5-D3DBD82D6691}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix filtering logic; add tests to verify
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632F723F-2A9F-4130-955A-91385D4B5910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A93399-A1B5-4B15-A366-A2AD52B1EBD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -28,6 +28,7 @@
     <definedName name="YesNo">YesNo!$A$1:$A$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="120">
   <si>
     <t>Name</t>
   </si>
@@ -362,18 +363,9 @@
     <t>Holiday &gt; Veterans Day</t>
   </si>
   <si>
-    <t>Quick Search &gt; Featured</t>
-  </si>
-  <si>
     <t>Quick Search &gt; New Designs</t>
   </si>
   <si>
-    <t>Event/Awareness &gt; Golf</t>
-  </si>
-  <si>
-    <t>Union Specific &gt; IAM</t>
-  </si>
-  <si>
     <t>Location Specific &gt; Oversize</t>
   </si>
   <si>
@@ -414,6 +406,9 @@
   </si>
   <si>
     <t>This sheet should not be edited.</t>
+  </si>
+  <si>
+    <t>Quick Search &gt; Best Sellers</t>
   </si>
 </sst>
 </file>
@@ -767,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,7 +787,7 @@
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -840,25 +835,25 @@
         <v>41</v>
       </c>
       <c r="Q1" t="s">
+        <v>112</v>
+      </c>
+      <c r="R1" t="s">
+        <v>114</v>
+      </c>
+      <c r="S1" t="s">
+        <v>113</v>
+      </c>
+      <c r="T1" t="s">
         <v>115</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
+        <v>116</v>
+      </c>
+      <c r="V1" t="s">
         <v>117</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>116</v>
-      </c>
-      <c r="T1" t="s">
-        <v>118</v>
-      </c>
-      <c r="U1" t="s">
-        <v>119</v>
-      </c>
-      <c r="V1" t="s">
-        <v>120</v>
-      </c>
-      <c r="W1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
@@ -881,7 +876,7 @@
         <v>103</v>
       </c>
       <c r="G2" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="K2" t="s">
         <v>14</v>
@@ -913,7 +908,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
@@ -948,13 +943,13 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
@@ -983,7 +978,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K5" t="s">
         <v>14</v>
@@ -1018,7 +1013,7 @@
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K6" t="s">
         <v>14</v>
@@ -1062,10 +1057,10 @@
         <v>17</v>
       </c>
       <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" t="s">
         <v>108</v>
-      </c>
-      <c r="G7" t="s">
-        <v>111</v>
       </c>
       <c r="K7" t="s">
         <v>14</v>
@@ -1097,7 +1092,7 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="K8" t="s">
         <v>15</v>
@@ -1129,10 +1124,10 @@
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G9" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="K9" t="s">
         <v>15</v>
@@ -1186,7 +1181,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1292,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1586536D-3214-4B71-B711-EFBAF2410143}">
   <dimension ref="A1:C52"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1322,7 +1317,7 @@
         <v>51</v>
       </c>
       <c r="C2" t="str">
-        <f>_xlfn.CONCAT(B2, " &gt; ", A2)</f>
+        <f t="shared" ref="C2:C33" si="0">_xlfn.CONCAT(B2, " &gt; ", A2)</f>
         <v>Quick Search &gt; New Designs</v>
       </c>
     </row>
@@ -1334,7 +1329,7 @@
         <v>51</v>
       </c>
       <c r="C3" t="str">
-        <f>_xlfn.CONCAT(B3, " &gt; ", A3)</f>
+        <f t="shared" si="0"/>
         <v>Quick Search &gt; Best Sellers</v>
       </c>
     </row>
@@ -1346,7 +1341,7 @@
         <v>51</v>
       </c>
       <c r="C4" t="str">
-        <f>_xlfn.CONCAT(B4, " &gt; ", A4)</f>
+        <f t="shared" si="0"/>
         <v>Quick Search &gt; Staff Favorites</v>
       </c>
     </row>
@@ -1358,7 +1353,7 @@
         <v>51</v>
       </c>
       <c r="C5" t="str">
-        <f>_xlfn.CONCAT(B5, " &gt; ", A5)</f>
+        <f t="shared" si="0"/>
         <v>Quick Search &gt; Classics</v>
       </c>
     </row>
@@ -1370,7 +1365,7 @@
         <v>51</v>
       </c>
       <c r="C6" t="str">
-        <f>_xlfn.CONCAT(B6, " &gt; ", A6)</f>
+        <f t="shared" si="0"/>
         <v>Quick Search &gt; Patriotic</v>
       </c>
     </row>
@@ -1382,7 +1377,7 @@
         <v>51</v>
       </c>
       <c r="C7" t="str">
-        <f>_xlfn.CONCAT(B7, " &gt; ", A7)</f>
+        <f t="shared" si="0"/>
         <v>Quick Search &gt; Economy</v>
       </c>
     </row>
@@ -1394,7 +1389,7 @@
         <v>51</v>
       </c>
       <c r="C8" t="str">
-        <f>_xlfn.CONCAT(B8, " &gt; ", A8)</f>
+        <f t="shared" si="0"/>
         <v>Quick Search &gt; Ladies</v>
       </c>
     </row>
@@ -1406,7 +1401,7 @@
         <v>52</v>
       </c>
       <c r="C9" t="str">
-        <f>_xlfn.CONCAT(B9, " &gt; ", A9)</f>
+        <f t="shared" si="0"/>
         <v>Event/Awareness &gt; Strike &amp; Negotiations</v>
       </c>
     </row>
@@ -1418,7 +1413,7 @@
         <v>52</v>
       </c>
       <c r="C10" t="str">
-        <f>_xlfn.CONCAT(B10, " &gt; ", A10)</f>
+        <f t="shared" si="0"/>
         <v>Event/Awareness &gt; Golf</v>
       </c>
     </row>
@@ -1430,7 +1425,7 @@
         <v>52</v>
       </c>
       <c r="C11" t="str">
-        <f>_xlfn.CONCAT(B11, " &gt; ", A11)</f>
+        <f t="shared" si="0"/>
         <v>Event/Awareness &gt; Picnics</v>
       </c>
     </row>
@@ -1442,7 +1437,7 @@
         <v>52</v>
       </c>
       <c r="C12" t="str">
-        <f>_xlfn.CONCAT(B12, " &gt; ", A12)</f>
+        <f t="shared" si="0"/>
         <v>Event/Awareness &gt; Anniversary</v>
       </c>
     </row>
@@ -1454,7 +1449,7 @@
         <v>52</v>
       </c>
       <c r="C13" t="str">
-        <f>_xlfn.CONCAT(B13, " &gt; ", A13)</f>
+        <f t="shared" si="0"/>
         <v>Event/Awareness &gt; Political</v>
       </c>
     </row>
@@ -1466,7 +1461,7 @@
         <v>52</v>
       </c>
       <c r="C14" t="str">
-        <f>_xlfn.CONCAT(B14, " &gt; ", A14)</f>
+        <f t="shared" si="0"/>
         <v>Event/Awareness &gt; Breast Cancer</v>
       </c>
     </row>
@@ -1478,7 +1473,7 @@
         <v>3</v>
       </c>
       <c r="C15" t="str">
-        <f>_xlfn.CONCAT(B15, " &gt; ", A15)</f>
+        <f t="shared" si="0"/>
         <v>Holiday &gt; Labor Day</v>
       </c>
     </row>
@@ -1490,7 +1485,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="str">
-        <f>_xlfn.CONCAT(B16, " &gt; ", A16)</f>
+        <f t="shared" si="0"/>
         <v>Holiday &gt; St. Patrick's Day</v>
       </c>
     </row>
@@ -1502,7 +1497,7 @@
         <v>3</v>
       </c>
       <c r="C17" t="str">
-        <f>_xlfn.CONCAT(B17, " &gt; ", A17)</f>
+        <f t="shared" si="0"/>
         <v>Holiday &gt; Veterans Day</v>
       </c>
     </row>
@@ -1514,7 +1509,7 @@
         <v>53</v>
       </c>
       <c r="C18" t="str">
-        <f>_xlfn.CONCAT(B18, " &gt; ", A18)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; International Logos</v>
       </c>
     </row>
@@ -1526,7 +1521,7 @@
         <v>53</v>
       </c>
       <c r="C19" t="str">
-        <f>_xlfn.CONCAT(B19, " &gt; ", A19)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; APWU</v>
       </c>
     </row>
@@ -1538,7 +1533,7 @@
         <v>53</v>
       </c>
       <c r="C20" t="str">
-        <f>_xlfn.CONCAT(B20, " &gt; ", A20)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; BAC</v>
       </c>
     </row>
@@ -1550,7 +1545,7 @@
         <v>53</v>
       </c>
       <c r="C21" t="str">
-        <f>_xlfn.CONCAT(B21, " &gt; ", A21)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; Boilermakers</v>
       </c>
     </row>
@@ -1562,7 +1557,7 @@
         <v>53</v>
       </c>
       <c r="C22" t="str">
-        <f>_xlfn.CONCAT(B22, " &gt; ", A22)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; Carpenters</v>
       </c>
     </row>
@@ -1574,7 +1569,7 @@
         <v>53</v>
       </c>
       <c r="C23" t="str">
-        <f>_xlfn.CONCAT(B23, " &gt; ", A23)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; CWA</v>
       </c>
     </row>
@@ -1586,7 +1581,7 @@
         <v>53</v>
       </c>
       <c r="C24" t="str">
-        <f>_xlfn.CONCAT(B24, " &gt; ", A24)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; Electrical Workers</v>
       </c>
     </row>
@@ -1598,7 +1593,7 @@
         <v>53</v>
       </c>
       <c r="C25" t="str">
-        <f>_xlfn.CONCAT(B25, " &gt; ", A25)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; IAFF</v>
       </c>
     </row>
@@ -1610,7 +1605,7 @@
         <v>53</v>
       </c>
       <c r="C26" t="str">
-        <f>_xlfn.CONCAT(B26, " &gt; ", A26)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; IAM</v>
       </c>
     </row>
@@ -1622,7 +1617,7 @@
         <v>53</v>
       </c>
       <c r="C27" t="str">
-        <f>_xlfn.CONCAT(B27, " &gt; ", A27)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; IATSE</v>
       </c>
     </row>
@@ -1634,7 +1629,7 @@
         <v>53</v>
       </c>
       <c r="C28" t="str">
-        <f>_xlfn.CONCAT(B28, " &gt; ", A28)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; Ironworkers</v>
       </c>
     </row>
@@ -1646,7 +1641,7 @@
         <v>53</v>
       </c>
       <c r="C29" t="str">
-        <f>_xlfn.CONCAT(B29, " &gt; ", A29)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; Heat &amp; Frost Insulators</v>
       </c>
     </row>
@@ -1658,7 +1653,7 @@
         <v>53</v>
       </c>
       <c r="C30" t="str">
-        <f>_xlfn.CONCAT(B30, " &gt; ", A30)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; IUEC</v>
       </c>
     </row>
@@ -1670,7 +1665,7 @@
         <v>53</v>
       </c>
       <c r="C31" t="str">
-        <f>_xlfn.CONCAT(B31, " &gt; ", A31)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; IUOE</v>
       </c>
     </row>
@@ -1682,7 +1677,7 @@
         <v>53</v>
       </c>
       <c r="C32" t="str">
-        <f>_xlfn.CONCAT(B32, " &gt; ", A32)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; IUPAT</v>
       </c>
     </row>
@@ -1694,7 +1689,7 @@
         <v>53</v>
       </c>
       <c r="C33" t="str">
-        <f>_xlfn.CONCAT(B33, " &gt; ", A33)</f>
+        <f t="shared" si="0"/>
         <v>Union Specific &gt; Laborers</v>
       </c>
     </row>
@@ -1706,7 +1701,7 @@
         <v>53</v>
       </c>
       <c r="C34" t="str">
-        <f>_xlfn.CONCAT(B34, " &gt; ", A34)</f>
+        <f t="shared" ref="C34:C65" si="1">_xlfn.CONCAT(B34, " &gt; ", A34)</f>
         <v>Union Specific &gt; Mailhandlers</v>
       </c>
     </row>
@@ -1718,7 +1713,7 @@
         <v>53</v>
       </c>
       <c r="C35" t="str">
-        <f>_xlfn.CONCAT(B35, " &gt; ", A35)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; NATCA</v>
       </c>
     </row>
@@ -1730,7 +1725,7 @@
         <v>53</v>
       </c>
       <c r="C36" t="str">
-        <f>_xlfn.CONCAT(B36, " &gt; ", A36)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; NALC</v>
       </c>
     </row>
@@ -1742,7 +1737,7 @@
         <v>53</v>
       </c>
       <c r="C37" t="str">
-        <f>_xlfn.CONCAT(B37, " &gt; ", A37)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; NEA</v>
       </c>
     </row>
@@ -1754,7 +1749,7 @@
         <v>53</v>
       </c>
       <c r="C38" t="str">
-        <f>_xlfn.CONCAT(B38, " &gt; ", A38)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; OPCMIA</v>
       </c>
     </row>
@@ -1766,7 +1761,7 @@
         <v>53</v>
       </c>
       <c r="C39" t="str">
-        <f>_xlfn.CONCAT(B39, " &gt; ", A39)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; OPEIU</v>
       </c>
     </row>
@@ -1778,7 +1773,7 @@
         <v>53</v>
       </c>
       <c r="C40" t="str">
-        <f>_xlfn.CONCAT(B40, " &gt; ", A40)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; PASS</v>
       </c>
     </row>
@@ -1790,7 +1785,7 @@
         <v>53</v>
       </c>
       <c r="C41" t="str">
-        <f>_xlfn.CONCAT(B41, " &gt; ", A41)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; Nurses</v>
       </c>
     </row>
@@ -1802,7 +1797,7 @@
         <v>53</v>
       </c>
       <c r="C42" t="str">
-        <f>_xlfn.CONCAT(B42, " &gt; ", A42)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; Roofers</v>
       </c>
     </row>
@@ -1814,7 +1809,7 @@
         <v>53</v>
       </c>
       <c r="C43" t="str">
-        <f>_xlfn.CONCAT(B43, " &gt; ", A43)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; SEIU</v>
       </c>
     </row>
@@ -1826,7 +1821,7 @@
         <v>53</v>
       </c>
       <c r="C44" t="str">
-        <f>_xlfn.CONCAT(B44, " &gt; ", A44)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; SMART</v>
       </c>
     </row>
@@ -1838,7 +1833,7 @@
         <v>53</v>
       </c>
       <c r="C45" t="str">
-        <f>_xlfn.CONCAT(B45, " &gt; ", A45)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; Teamsters</v>
       </c>
     </row>
@@ -1850,7 +1845,7 @@
         <v>53</v>
       </c>
       <c r="C46" t="str">
-        <f>_xlfn.CONCAT(B46, " &gt; ", A46)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; UA</v>
       </c>
     </row>
@@ -1862,7 +1857,7 @@
         <v>53</v>
       </c>
       <c r="C47" t="str">
-        <f>_xlfn.CONCAT(B47, " &gt; ", A47)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; UAW</v>
       </c>
     </row>
@@ -1874,7 +1869,7 @@
         <v>53</v>
       </c>
       <c r="C48" t="str">
-        <f>_xlfn.CONCAT(B48, " &gt; ", A48)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; UWUA</v>
       </c>
     </row>
@@ -1886,7 +1881,7 @@
         <v>53</v>
       </c>
       <c r="C49" t="str">
-        <f>_xlfn.CONCAT(B49, " &gt; ", A49)</f>
+        <f t="shared" si="1"/>
         <v>Union Specific &gt; USW</v>
       </c>
     </row>
@@ -1898,7 +1893,7 @@
         <v>54</v>
       </c>
       <c r="C50" t="str">
-        <f>_xlfn.CONCAT(B50, " &gt; ", A50)</f>
+        <f t="shared" si="1"/>
         <v>Location Specific &gt; Sleeve</v>
       </c>
     </row>
@@ -1910,7 +1905,7 @@
         <v>54</v>
       </c>
       <c r="C51" t="str">
-        <f>_xlfn.CONCAT(B51, " &gt; ", A51)</f>
+        <f t="shared" si="1"/>
         <v>Location Specific &gt; Oversize</v>
       </c>
     </row>
@@ -1922,7 +1917,7 @@
         <v>54</v>
       </c>
       <c r="C52" t="str">
-        <f>_xlfn.CONCAT(B52, " &gt; ", A52)</f>
+        <f t="shared" si="1"/>
         <v>Location Specific &gt; Youth/Kids</v>
       </c>
     </row>
@@ -1958,7 +1953,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add design type field to categories
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEDB93D-8904-4B7D-B35B-3E798619771F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E699F8-55C6-4DC9-B606-5F5DB65949C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Designs" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <definedName name="YesNo">YesNo!$A$1:$A$2</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -430,6 +429,24 @@
   </si>
   <si>
     <t>Skull With Flag</t>
+  </si>
+  <si>
+    <t>International Union Logos</t>
+  </si>
+  <si>
+    <t>Inspiration Board</t>
+  </si>
+  <si>
+    <t>Hats/Beanies</t>
+  </si>
+  <si>
+    <t>Chest/Sleeve</t>
+  </si>
+  <si>
+    <t>Full Size Embroidery</t>
+  </si>
+  <si>
+    <t>Mixed Media/Dye Sublimation/Applique</t>
   </si>
 </sst>
 </file>
@@ -783,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
   <dimension ref="A1:W16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1460,48 +1477,87 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE8B92B-2F2F-44F6-BB2D-490F7DE9352F}">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{D48885AF-71A2-4010-BC40-884B7D029D0C}">
+      <formula1>DesignType</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1509,17 +1565,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1586536D-3214-4B71-B711-EFBAF2410143}">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1925,7 +1981,7 @@
         <v>53</v>
       </c>
       <c r="C34" t="str">
-        <f t="shared" ref="C34:C52" si="1">_xlfn.CONCAT(B34, " &gt; ", A34)</f>
+        <f t="shared" ref="C34:C87" si="1">_xlfn.CONCAT(B34, " &gt; ", A34)</f>
         <v>Union Specific &gt; Mailhandlers</v>
       </c>
     </row>
@@ -2145,9 +2201,429 @@
         <v>Location Specific &gt; Youth/Kids</v>
       </c>
     </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; APWU</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>72</v>
+      </c>
+      <c r="B54" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; BAC</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>73</v>
+      </c>
+      <c r="B55" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Boilermakers</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>74</v>
+      </c>
+      <c r="B56" t="s">
+        <v>127</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Carpenters</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>75</v>
+      </c>
+      <c r="B57" t="s">
+        <v>127</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; CWA</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Electrical Workers</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>77</v>
+      </c>
+      <c r="B59" t="s">
+        <v>127</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; IAFF</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>78</v>
+      </c>
+      <c r="B60" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; IAM</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>79</v>
+      </c>
+      <c r="B61" t="s">
+        <v>127</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; IATSE</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>80</v>
+      </c>
+      <c r="B62" t="s">
+        <v>127</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Ironworkers</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Heat &amp; Frost Insulators</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; IUEC</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>83</v>
+      </c>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; IUOE</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>19</v>
+      </c>
+      <c r="B66" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; IUPAT</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>84</v>
+      </c>
+      <c r="B67" t="s">
+        <v>127</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Laborers</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>85</v>
+      </c>
+      <c r="B68" t="s">
+        <v>127</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Mailhandlers</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69" t="s">
+        <v>127</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; NATCA</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>87</v>
+      </c>
+      <c r="B70" t="s">
+        <v>127</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; NALC</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>88</v>
+      </c>
+      <c r="B71" t="s">
+        <v>127</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; NEA</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>89</v>
+      </c>
+      <c r="B72" t="s">
+        <v>127</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; OPCMIA</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>90</v>
+      </c>
+      <c r="B73" t="s">
+        <v>127</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; OPEIU</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>91</v>
+      </c>
+      <c r="B74" t="s">
+        <v>127</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; PASS</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" t="s">
+        <v>127</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Nurses</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>93</v>
+      </c>
+      <c r="B76" t="s">
+        <v>127</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Roofers</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>18</v>
+      </c>
+      <c r="B77" t="s">
+        <v>127</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; SEIU</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78" t="s">
+        <v>127</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; SMART</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>95</v>
+      </c>
+      <c r="B79" t="s">
+        <v>127</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; Teamsters</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" t="s">
+        <v>127</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; UA</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>97</v>
+      </c>
+      <c r="B81" t="s">
+        <v>127</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; UAW</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>98</v>
+      </c>
+      <c r="B82" t="s">
+        <v>127</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; UWUA</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83" t="s">
+        <v>127</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="1"/>
+        <v>International Union Logos &gt; USW</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>129</v>
+      </c>
+      <c r="B84" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="1"/>
+        <v>Inspiration Board &gt; Hats/Beanies</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>130</v>
+      </c>
+      <c r="B85" t="s">
+        <v>128</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="1"/>
+        <v>Inspiration Board &gt; Chest/Sleeve</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>131</v>
+      </c>
+      <c r="B86" t="s">
+        <v>128</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="1"/>
+        <v>Inspiration Board &gt; Full Size Embroidery</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>132</v>
+      </c>
+      <c r="B87" t="s">
+        <v>128</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="1"/>
+        <v>Inspiration Board &gt; Mixed Media/Dye Sublimation/Applique</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B54:B1048576 B2:B52" xr:uid="{2E446173-9549-4294-9E21-30D2EFE6849D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B1048576" xr:uid="{2E446173-9549-4294-9E21-30D2EFE6849D}">
       <formula1>Categories</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fix filtering logic so that the first design is no longer filtered out by default; update sample db and tests to reflect the new data model
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,21 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B06870-F568-4435-8D04-60AFA50F1E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D081ACA-406F-4C07-8ADA-54941748D492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2595" yWindow="1890" windowWidth="21600" windowHeight="11235" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Designs" sheetId="1" r:id="rId1"/>
-    <sheet name="DesignType" sheetId="6" r:id="rId2"/>
-    <sheet name="Tags" sheetId="5" r:id="rId3"/>
-    <sheet name="Categories" sheetId="2" r:id="rId4"/>
-    <sheet name="Subcategories" sheetId="3" r:id="rId5"/>
+    <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
+    <sheet name="Embroidery Designs" sheetId="1" r:id="rId2"/>
+    <sheet name="Categories" sheetId="2" r:id="rId3"/>
+    <sheet name="Subcategories" sheetId="3" r:id="rId4"/>
+    <sheet name="Status" sheetId="8" r:id="rId5"/>
     <sheet name="YesNo" sheetId="4" r:id="rId6"/>
+    <sheet name="Tags" sheetId="5" r:id="rId7"/>
+    <sheet name="DesignType" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="Categories">Categories!$A$2:$A$1048576</definedName>
     <definedName name="DesignType">DesignType!$A$1:$A$2</definedName>
+    <definedName name="Status">Status!$A$1:$A$2</definedName>
     <definedName name="Subcategories">Subcategories!$C$2:$C$1048576</definedName>
     <definedName name="Tags">Tags!$A$2:$A$1048576</definedName>
     <definedName name="YesNo">YesNo!$A$1:$A$2</definedName>
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="149">
   <si>
     <t>Name</t>
   </si>
@@ -447,16 +450,70 @@
   </si>
   <si>
     <t>Mixed Media/Dye Sublimation/Applique</t>
+  </si>
+  <si>
+    <t>Tag6</t>
+  </si>
+  <si>
+    <t>Tag7</t>
+  </si>
+  <si>
+    <t>Tag8</t>
+  </si>
+  <si>
+    <t>Tag9</t>
+  </si>
+  <si>
+    <t>Tag10</t>
+  </si>
+  <si>
+    <t>Tag11</t>
+  </si>
+  <si>
+    <t>Tag12</t>
+  </si>
+  <si>
+    <t>Tag13</t>
+  </si>
+  <si>
+    <t>Tag14</t>
+  </si>
+  <si>
+    <t>Tag15</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Dropbox Image Path 7</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Image To Use</t>
+  </si>
+  <si>
+    <t>Published</t>
+  </si>
+  <si>
+    <t>Draft</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -797,11 +854,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
-  <dimension ref="A1:W16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
+  <dimension ref="A1:AJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,15 +873,15 @@
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="17" max="17" width="71.85546875" customWidth="1"/>
-    <col min="18" max="18" width="63.85546875" customWidth="1"/>
-    <col min="19" max="19" width="59.42578125" customWidth="1"/>
-    <col min="20" max="20" width="60.140625" customWidth="1"/>
-    <col min="21" max="21" width="61.42578125" customWidth="1"/>
-    <col min="22" max="22" width="57.85546875" customWidth="1"/>
+    <col min="29" max="29" width="71.85546875" customWidth="1"/>
+    <col min="30" max="30" width="63.85546875" customWidth="1"/>
+    <col min="31" max="31" width="59.42578125" customWidth="1"/>
+    <col min="32" max="32" width="60.140625" customWidth="1"/>
+    <col min="33" max="33" width="61.42578125" customWidth="1"/>
+    <col min="34" max="34" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>111</v>
       </c>
@@ -873,28 +931,67 @@
         <v>41</v>
       </c>
       <c r="Q1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R1" t="s">
+        <v>134</v>
+      </c>
+      <c r="S1" t="s">
+        <v>135</v>
+      </c>
+      <c r="T1" t="s">
+        <v>136</v>
+      </c>
+      <c r="U1" t="s">
+        <v>137</v>
+      </c>
+      <c r="V1" t="s">
+        <v>138</v>
+      </c>
+      <c r="W1" t="s">
+        <v>139</v>
+      </c>
+      <c r="X1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC1" t="s">
         <v>112</v>
       </c>
-      <c r="R1" t="s">
+      <c r="AD1" t="s">
         <v>114</v>
       </c>
-      <c r="S1" t="s">
+      <c r="AE1" t="s">
         <v>113</v>
       </c>
-      <c r="T1" t="s">
+      <c r="AF1" t="s">
         <v>115</v>
       </c>
-      <c r="U1" t="s">
+      <c r="AG1" t="s">
         <v>116</v>
       </c>
-      <c r="V1" t="s">
+      <c r="AH1" t="s">
         <v>117</v>
       </c>
-      <c r="W1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="AI1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1025</v>
       </c>
@@ -922,22 +1019,22 @@
       <c r="L2" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="AC2" t="s">
         <v>42</v>
       </c>
-      <c r="R2" t="s">
+      <c r="AD2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1009</v>
+        <v>1003</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>29</v>
@@ -946,453 +1043,617 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
+        <v>108</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1012</v>
+      </c>
+      <c r="B6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1013</v>
+      </c>
+      <c r="B7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1014</v>
+      </c>
+      <c r="B8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1015</v>
+      </c>
+      <c r="B9" t="s">
+        <v>123</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1016</v>
+      </c>
+      <c r="B10" t="s">
+        <v>124</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1017</v>
+      </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1018</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L12" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{A61431EB-F298-41CC-8A14-D29D28DE34A1}">
+      <formula1>DesignType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Z1048576" xr:uid="{0F9108B0-AF43-4436-8202-F35401506D80}">
+      <formula1>Tags</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:J1048576" xr:uid="{358D683C-DBF6-4E6F-8311-F37F9C488CA5}">
+      <formula1>Subcategories</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{377959F3-1E32-48D5-BD0D-DAFF6699BAE0}">
+      <formula1>YesNo</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1048576" xr:uid="{99999286-3ED4-4B5C-B2BF-6EDC933F7B52}">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
+  <dimension ref="A1:AJ5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M23" sqref="M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="90.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="29" max="29" width="71.85546875" customWidth="1"/>
+    <col min="30" max="30" width="63.85546875" customWidth="1"/>
+    <col min="31" max="31" width="59.42578125" customWidth="1"/>
+    <col min="32" max="32" width="60.140625" customWidth="1"/>
+    <col min="33" max="33" width="61.42578125" customWidth="1"/>
+    <col min="34" max="34" width="23.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" t="s">
+        <v>40</v>
+      </c>
+      <c r="P1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>133</v>
+      </c>
+      <c r="R1" t="s">
+        <v>134</v>
+      </c>
+      <c r="S1" t="s">
+        <v>135</v>
+      </c>
+      <c r="T1" t="s">
+        <v>136</v>
+      </c>
+      <c r="U1" t="s">
+        <v>137</v>
+      </c>
+      <c r="V1" t="s">
+        <v>138</v>
+      </c>
+      <c r="W1" t="s">
+        <v>139</v>
+      </c>
+      <c r="X1" t="s">
+        <v>140</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>141</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1009</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
         <v>119</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1006</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" t="s">
+        <v>110</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
       </c>
       <c r="L3" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>43</v>
-      </c>
-      <c r="R3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC3" t="s">
         <v>44</v>
       </c>
-      <c r="S3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1006</v>
+        <v>1000</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D4" t="s">
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
-      </c>
-      <c r="G4" t="s">
         <v>106</v>
-      </c>
-      <c r="H4" t="s">
-        <v>110</v>
       </c>
       <c r="K4" t="s">
         <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>107</v>
+      </c>
+      <c r="G5" t="s">
+        <v>109</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M5" t="s">
-        <v>33</v>
-      </c>
-      <c r="N5" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>46</v>
-      </c>
-      <c r="R6" t="s">
-        <v>44</v>
-      </c>
-      <c r="S6" t="s">
-        <v>43</v>
-      </c>
-      <c r="T6" t="s">
-        <v>48</v>
-      </c>
-      <c r="U6" t="s">
-        <v>47</v>
-      </c>
-      <c r="V6" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC5" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>105</v>
-      </c>
-      <c r="G7" t="s">
-        <v>108</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>33</v>
-      </c>
-      <c r="M7" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1000</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>106</v>
-      </c>
-      <c r="K8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L8" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>48</v>
-      </c>
-      <c r="R8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>1001</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>107</v>
-      </c>
-      <c r="G9" t="s">
-        <v>109</v>
-      </c>
-      <c r="K9" t="s">
-        <v>15</v>
-      </c>
-      <c r="L9" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>1012</v>
-      </c>
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" t="s">
-        <v>104</v>
-      </c>
-      <c r="K10" t="s">
-        <v>14</v>
-      </c>
-      <c r="L10" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1013</v>
-      </c>
-      <c r="B11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" t="s">
-        <v>104</v>
-      </c>
-      <c r="K11" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1014</v>
-      </c>
-      <c r="B12" t="s">
-        <v>122</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>104</v>
-      </c>
-      <c r="K12" t="s">
-        <v>14</v>
-      </c>
-      <c r="L12" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1015</v>
-      </c>
-      <c r="B13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>104</v>
-      </c>
-      <c r="K13" t="s">
-        <v>14</v>
-      </c>
-      <c r="L13" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1016</v>
-      </c>
-      <c r="B14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" t="s">
-        <v>104</v>
-      </c>
-      <c r="K14" t="s">
-        <v>14</v>
-      </c>
-      <c r="L14" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1017</v>
-      </c>
-      <c r="B15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s">
-        <v>104</v>
-      </c>
-      <c r="K15" t="s">
-        <v>14</v>
-      </c>
-      <c r="L15" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1018</v>
-      </c>
-      <c r="B16" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s">
-        <v>104</v>
-      </c>
-      <c r="K16" t="s">
-        <v>14</v>
-      </c>
-      <c r="L16" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>45</v>
-      </c>
-    </row>
   </sheetData>
-  <dataValidations count="4">
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
       <formula1>YesNo</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:J1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
       <formula1>Subcategories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:P1048576" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Z1048576" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
       <formula1>Tags</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{D0466454-C892-488E-AA3C-A206F5B6F670}">
       <formula1>DesignType</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1048576" xr:uid="{9EF19CFE-4BEB-4B6E-9893-F1BFEBCAA2B4}">
+      <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1400,82 +1661,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A83CC9-1574-4180-85AD-01F92A9D1604}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096F644A-6816-46A6-9C37-F543D22E3BF1}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE8B92B-2F2F-44F6-BB2D-490F7DE9352F}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -1563,7 +1749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1586536D-3214-4B71-B711-EFBAF2410143}">
   <dimension ref="A1:C87"/>
   <sheetViews>
@@ -2631,8 +2817,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBDC08E-FD24-497A-86A5-D3DBD82D6691}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8207F966-3498-4646-82AC-E7F049D20E38}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2643,12 +2829,117 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBDC08E-FD24-497A-86A5-D3DBD82D6691}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096F644A-6816-46A6-9C37-F543D22E3BF1}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A83CC9-1574-4180-85AD-01F92A9D1604}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add option to return all designs with the same design number as a specific design
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D081ACA-406F-4C07-8ADA-54941748D492}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F422F7-467D-4217-9FE4-A32C40F780D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -498,6 +498,42 @@
   </si>
   <si>
     <t>Draft</t>
+  </si>
+  <si>
+    <t>Union Swirl</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; IAM</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; IUEC</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; Laborers</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; UAW</t>
+  </si>
+  <si>
+    <t>Union Specific &gt; USW</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205.jpg</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (2).jpg</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (3).jpg</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (4).jpg</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (5).jpg</t>
   </si>
 </sst>
 </file>
@@ -857,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
   <dimension ref="A1:AJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
     </sheetView>
@@ -1367,11 +1403,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
-  <dimension ref="A1:AJ5"/>
+  <dimension ref="A1:AJ10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC16" sqref="AC16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,6 +1671,136 @@
       </c>
       <c r="AC5" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>151</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L6" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>205</v>
+      </c>
+      <c r="B7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" t="s">
+        <v>150</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>152</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>205</v>
+      </c>
+      <c r="B8" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K8" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>205</v>
+      </c>
+      <c r="B9" t="s">
+        <v>149</v>
+      </c>
+      <c r="D9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>154</v>
+      </c>
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>205</v>
+      </c>
+      <c r="B10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D10" t="s">
+        <v>150</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>155</v>
+      </c>
+      <c r="K10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L10" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Always filter out draft designs
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F422F7-467D-4217-9FE4-A32C40F780D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4734541C-8C66-4C5A-9402-A9EED99D8C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -534,6 +534,12 @@
   </si>
   <si>
     <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (5).jpg</t>
+  </si>
+  <si>
+    <t>Draft Design</t>
+  </si>
+  <si>
+    <t>Inspiration Board &gt; Hats/Beanies</t>
   </si>
 </sst>
 </file>
@@ -894,8 +900,8 @@
   <dimension ref="A1:AJ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G5" sqref="G5"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB2" sqref="AB2:AB12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,6 +1061,9 @@
       <c r="L2" t="s">
         <v>35</v>
       </c>
+      <c r="AB2" t="s">
+        <v>147</v>
+      </c>
       <c r="AC2" t="s">
         <v>42</v>
       </c>
@@ -1093,6 +1102,9 @@
       <c r="N3" t="s">
         <v>35</v>
       </c>
+      <c r="AB3" t="s">
+        <v>147</v>
+      </c>
       <c r="AC3" t="s">
         <v>45</v>
       </c>
@@ -1122,6 +1134,9 @@
       <c r="L4" t="s">
         <v>33</v>
       </c>
+      <c r="AB4" t="s">
+        <v>147</v>
+      </c>
       <c r="AC4" t="s">
         <v>46</v>
       </c>
@@ -1172,6 +1187,9 @@
       <c r="M5" t="s">
         <v>32</v>
       </c>
+      <c r="AB5" t="s">
+        <v>147</v>
+      </c>
       <c r="AC5" t="s">
         <v>47</v>
       </c>
@@ -1201,6 +1219,9 @@
       <c r="L6" t="s">
         <v>33</v>
       </c>
+      <c r="AB6" t="s">
+        <v>147</v>
+      </c>
       <c r="AC6" t="s">
         <v>47</v>
       </c>
@@ -1230,6 +1251,9 @@
       <c r="L7" t="s">
         <v>32</v>
       </c>
+      <c r="AB7" t="s">
+        <v>147</v>
+      </c>
       <c r="AC7" t="s">
         <v>45</v>
       </c>
@@ -1259,6 +1283,9 @@
       <c r="L8" t="s">
         <v>32</v>
       </c>
+      <c r="AB8" t="s">
+        <v>147</v>
+      </c>
       <c r="AC8" t="s">
         <v>45</v>
       </c>
@@ -1288,6 +1315,9 @@
       <c r="L9" t="s">
         <v>35</v>
       </c>
+      <c r="AB9" t="s">
+        <v>147</v>
+      </c>
       <c r="AC9" t="s">
         <v>49</v>
       </c>
@@ -1317,6 +1347,9 @@
       <c r="L10" t="s">
         <v>34</v>
       </c>
+      <c r="AB10" t="s">
+        <v>147</v>
+      </c>
       <c r="AC10" t="s">
         <v>47</v>
       </c>
@@ -1346,6 +1379,9 @@
       <c r="L11" t="s">
         <v>36</v>
       </c>
+      <c r="AB11" t="s">
+        <v>147</v>
+      </c>
       <c r="AC11" t="s">
         <v>49</v>
       </c>
@@ -1374,6 +1410,9 @@
       </c>
       <c r="L12" t="s">
         <v>32</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>147</v>
       </c>
       <c r="AC12" t="s">
         <v>45</v>
@@ -1403,11 +1442,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
-  <dimension ref="A1:AJ10"/>
+  <dimension ref="A1:AJ11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC16" sqref="AC16"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC26" sqref="AC26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1564,6 +1603,9 @@
       <c r="L2" t="s">
         <v>34</v>
       </c>
+      <c r="AB2" t="s">
+        <v>147</v>
+      </c>
       <c r="AC2" t="s">
         <v>43</v>
       </c>
@@ -1605,6 +1647,9 @@
       <c r="L3" t="s">
         <v>33</v>
       </c>
+      <c r="AB3" t="s">
+        <v>147</v>
+      </c>
       <c r="AC3" t="s">
         <v>44</v>
       </c>
@@ -1634,6 +1679,9 @@
       <c r="L4" t="s">
         <v>36</v>
       </c>
+      <c r="AB4" t="s">
+        <v>147</v>
+      </c>
       <c r="AC4" t="s">
         <v>48</v>
       </c>
@@ -1669,6 +1717,9 @@
       <c r="L5" t="s">
         <v>36</v>
       </c>
+      <c r="AB5" t="s">
+        <v>147</v>
+      </c>
       <c r="AC5" t="s">
         <v>49</v>
       </c>
@@ -1695,6 +1746,9 @@
       <c r="L6" t="s">
         <v>34</v>
       </c>
+      <c r="AB6" t="s">
+        <v>147</v>
+      </c>
       <c r="AC6" t="s">
         <v>156</v>
       </c>
@@ -1721,6 +1775,9 @@
       <c r="L7" t="s">
         <v>34</v>
       </c>
+      <c r="AB7" t="s">
+        <v>147</v>
+      </c>
       <c r="AC7" t="s">
         <v>157</v>
       </c>
@@ -1747,6 +1804,9 @@
       <c r="L8" t="s">
         <v>34</v>
       </c>
+      <c r="AB8" t="s">
+        <v>147</v>
+      </c>
       <c r="AC8" t="s">
         <v>158</v>
       </c>
@@ -1773,6 +1833,9 @@
       <c r="L9" t="s">
         <v>34</v>
       </c>
+      <c r="AB9" t="s">
+        <v>147</v>
+      </c>
       <c r="AC9" t="s">
         <v>159</v>
       </c>
@@ -1799,7 +1862,36 @@
       <c r="L10" t="s">
         <v>34</v>
       </c>
+      <c r="AB10" t="s">
+        <v>147</v>
+      </c>
       <c r="AC10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+      <c r="D11" t="s">
+        <v>150</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>162</v>
+      </c>
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC11" t="s">
         <v>160</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add non-standard-size design to sample data; adjust tests accordingly
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4734541C-8C66-4C5A-9402-A9EED99D8C32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA46F75C-2FB0-45F1-BA0B-9C9097F8CF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -540,6 +540,18 @@
   </si>
   <si>
     <t>Inspiration Board &gt; Hats/Beanies</t>
+  </si>
+  <si>
+    <t>Oversize Design</t>
+  </si>
+  <si>
+    <t>#000001</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/549 (Oversize).jpg</t>
+  </si>
+  <si>
+    <t>Location Specific &gt; Sleeve</t>
   </si>
 </sst>
 </file>
@@ -897,11 +909,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
-  <dimension ref="A1:AJ12"/>
+  <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB2" sqref="AB2:AB12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1416,6 +1428,32 @@
       </c>
       <c r="AC12" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>549</v>
+      </c>
+      <c r="B13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D13" t="s">
+        <v>164</v>
+      </c>
+      <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>166</v>
+      </c>
+      <c r="L13" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>147</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1444,9 +1482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC26" sqref="AC26"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1898,19 +1936,19 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11 E13:E1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:J1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:J11 F13:J1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
       <formula1>Subcategories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Z1048576" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Z11 L13:Z1048576" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
       <formula1>Tags</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{D0466454-C892-488E-AA3C-A206F5B6F670}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K11 K13:K1048576" xr:uid="{D0466454-C892-488E-AA3C-A206F5B6F670}">
       <formula1>DesignType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1048576" xr:uid="{9EF19CFE-4BEB-4B6E-9893-F1BFEBCAA2B4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB11 AB13:AB1048576" xr:uid="{9EF19CFE-4BEB-4B6E-9893-F1BFEBCAA2B4}">
       <formula1>Status</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Adjust column names for subcategory 1 and 2
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA46F75C-2FB0-45F1-BA0B-9C9097F8CF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD75141B-2DE4-49B4-BA7C-561AE0389696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -80,12 +80,6 @@
     <t>Labor Day</t>
   </si>
   <si>
-    <t>Subcategory1</t>
-  </si>
-  <si>
-    <t>Subcategory2</t>
-  </si>
-  <si>
     <t>Subcategory3</t>
   </si>
   <si>
@@ -552,6 +546,12 @@
   </si>
   <si>
     <t>Location Specific &gt; Sleeve</t>
+  </si>
+  <si>
+    <t>Subcategory1 - Union</t>
+  </si>
+  <si>
+    <t>Subcategory2 - Holiday/Event</t>
   </si>
 </sst>
 </file>
@@ -911,9 +911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A14" sqref="A14"/>
+      <selection pane="topRight" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,8 +923,8 @@
     <col min="3" max="3" width="90.140625" customWidth="1"/>
     <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
     <col min="29" max="29" width="71.85546875" customWidth="1"/>
@@ -937,7 +937,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -949,100 +949,100 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
       <c r="K1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" t="s">
-        <v>41</v>
-      </c>
       <c r="Q1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" t="s">
         <v>133</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>134</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>135</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>136</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>137</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>138</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>139</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>140</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>141</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI1" t="s">
         <v>142</v>
       </c>
-      <c r="AA1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>144</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1053,34 +1053,34 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AB2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AD2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1088,37 +1088,37 @@
         <v>1003</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N3" t="s">
         <v>33</v>
       </c>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
       <c r="AB3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
@@ -1126,46 +1126,46 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AB4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF4" t="s">
         <v>46</v>
       </c>
-      <c r="AD4" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>43</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>48</v>
-      </c>
       <c r="AG4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH4" t="s">
         <v>47</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -1173,37 +1173,37 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
-        <v>29</v>
-      </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="M5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AB5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -1211,31 +1211,31 @@
         <v>1012</v>
       </c>
       <c r="B6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AB6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -1243,31 +1243,31 @@
         <v>1013</v>
       </c>
       <c r="B7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" t="s">
-        <v>104</v>
-      </c>
-      <c r="K7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>32</v>
-      </c>
       <c r="AB7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -1275,31 +1275,31 @@
         <v>1014</v>
       </c>
       <c r="B8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AB8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -1307,31 +1307,31 @@
         <v>1015</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="AB9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -1339,31 +1339,31 @@
         <v>1016</v>
       </c>
       <c r="B10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -1371,31 +1371,31 @@
         <v>1017</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
-        <v>29</v>
-      </c>
       <c r="E11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AB11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
@@ -1403,31 +1403,31 @@
         <v>1018</v>
       </c>
       <c r="B12" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="L12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="AB12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
@@ -1435,25 +1435,25 @@
         <v>549</v>
       </c>
       <c r="B13" t="s">
+        <v>161</v>
+      </c>
+      <c r="D13" t="s">
+        <v>162</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" t="s">
+        <v>164</v>
+      </c>
+      <c r="L13" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC13" t="s">
         <v>163</v>
-      </c>
-      <c r="D13" t="s">
-        <v>164</v>
-      </c>
-      <c r="E13" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" t="s">
-        <v>166</v>
-      </c>
-      <c r="L13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>147</v>
-      </c>
-      <c r="AC13" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1482,9 +1482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A12" sqref="A12:XFD12"/>
+      <selection pane="topRight" activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1508,7 +1508,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1520,100 +1520,100 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" t="s">
+        <v>166</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
-      </c>
       <c r="K1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" t="s">
         <v>37</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>38</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>39</v>
       </c>
-      <c r="O1" t="s">
-        <v>40</v>
-      </c>
-      <c r="P1" t="s">
-        <v>41</v>
-      </c>
       <c r="Q1" t="s">
+        <v>131</v>
+      </c>
+      <c r="R1" t="s">
+        <v>132</v>
+      </c>
+      <c r="S1" t="s">
         <v>133</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>134</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>135</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>136</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>137</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>138</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>139</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>140</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>141</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AI1" t="s">
         <v>142</v>
       </c>
-      <c r="AA1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>116</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>117</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>144</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1624,34 +1624,34 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AD2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AE2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1662,34 +1662,34 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
         <v>104</v>
       </c>
-      <c r="G3" t="s">
-        <v>106</v>
-      </c>
       <c r="H3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="AB3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
@@ -1697,34 +1697,34 @@
         <v>1000</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AB4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="AD4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -1732,34 +1732,34 @@
         <v>1001</v>
       </c>
       <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G5" t="s">
         <v>107</v>
       </c>
-      <c r="G5" t="s">
-        <v>109</v>
-      </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="AB5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -1767,28 +1767,28 @@
         <v>205</v>
       </c>
       <c r="B6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
         <v>149</v>
       </c>
-      <c r="D6" t="s">
-        <v>150</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" t="s">
-        <v>151</v>
-      </c>
       <c r="K6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -1796,28 +1796,28 @@
         <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D7" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
         <v>150</v>
       </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>152</v>
-      </c>
       <c r="K7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -1825,28 +1825,28 @@
         <v>205</v>
       </c>
       <c r="B8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="K8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -1854,28 +1854,28 @@
         <v>205</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -1883,28 +1883,28 @@
         <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="K10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="AC10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -1912,25 +1912,25 @@
         <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="L11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AB11" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AC11" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -1975,23 +1975,23 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1999,39 +1999,39 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2068,15 +2068,15 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C33" si="0">_xlfn.CONCAT(B2, " &gt; ", A2)</f>
@@ -2085,10 +2085,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -2097,10 +2097,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -2109,10 +2109,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -2121,10 +2121,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -2133,10 +2133,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -2145,10 +2145,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2157,10 +2157,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -2169,10 +2169,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -2181,10 +2181,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -2193,10 +2193,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2205,10 +2205,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -2217,10 +2217,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -2241,7 +2241,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -2253,7 +2253,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -2265,10 +2265,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -2277,10 +2277,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -2289,10 +2289,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -2301,10 +2301,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -2313,10 +2313,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -2325,10 +2325,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -2337,10 +2337,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -2349,10 +2349,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -2361,10 +2361,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -2373,10 +2373,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -2385,10 +2385,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B28" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -2397,10 +2397,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -2409,10 +2409,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -2421,10 +2421,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -2433,10 +2433,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -2445,10 +2445,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -2457,10 +2457,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" ref="C34:C87" si="1">_xlfn.CONCAT(B34, " &gt; ", A34)</f>
@@ -2469,10 +2469,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
@@ -2481,10 +2481,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B36" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
@@ -2493,10 +2493,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
@@ -2505,10 +2505,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
@@ -2517,10 +2517,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
@@ -2529,10 +2529,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B40" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
@@ -2541,10 +2541,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
@@ -2553,10 +2553,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
@@ -2565,10 +2565,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
@@ -2577,10 +2577,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
@@ -2589,10 +2589,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
@@ -2601,10 +2601,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
@@ -2613,10 +2613,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
@@ -2625,10 +2625,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
@@ -2637,10 +2637,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
@@ -2649,10 +2649,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
@@ -2661,10 +2661,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
@@ -2673,10 +2673,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
@@ -2685,10 +2685,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
@@ -2697,10 +2697,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -2709,10 +2709,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B55" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -2721,10 +2721,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -2733,10 +2733,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B57" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
@@ -2745,10 +2745,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -2757,10 +2757,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -2769,10 +2769,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -2781,10 +2781,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
@@ -2793,10 +2793,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
@@ -2805,10 +2805,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B63" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
@@ -2817,10 +2817,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
@@ -2829,10 +2829,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B65" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
@@ -2841,10 +2841,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
@@ -2853,10 +2853,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="1"/>
@@ -2865,10 +2865,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -2877,10 +2877,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -2889,10 +2889,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -2901,10 +2901,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -2913,10 +2913,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -2925,10 +2925,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -2937,10 +2937,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -2949,10 +2949,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -2961,10 +2961,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -2973,10 +2973,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -2985,10 +2985,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -2997,10 +2997,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -3009,10 +3009,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B80" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
@@ -3021,10 +3021,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
@@ -3033,10 +3033,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B82" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
@@ -3045,10 +3045,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
@@ -3057,10 +3057,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B84" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
@@ -3069,10 +3069,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B85" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
@@ -3081,10 +3081,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B86" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -3093,10 +3093,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B87" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -3125,17 +3125,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3155,17 +3155,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -3190,27 +3190,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3230,17 +3230,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve design number sorting; make classification of new/classic designs based on date
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD75141B-2DE4-49B4-BA7C-561AE0389696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C498D89C-D650-4631-AB54-4D8303A7EB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -365,9 +365,6 @@
     <t>Location Specific &gt; Oversize</t>
   </si>
   <si>
-    <t>Quick Search &gt; Classics</t>
-  </si>
-  <si>
     <t>Union Specific &gt; International Logos</t>
   </si>
   <si>
@@ -552,6 +549,9 @@
   </si>
   <si>
     <t>Subcategory2 - Holiday/Event</t>
+  </si>
+  <si>
+    <t>1/1/2024</t>
   </si>
 </sst>
 </file>
@@ -593,8 +593,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,8 +913,8 @@
   <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G1" sqref="G1"/>
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA2" sqref="AA2:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,6 +928,7 @@
     <col min="7" max="7" width="29.5703125" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="1"/>
     <col min="29" max="29" width="71.85546875" customWidth="1"/>
     <col min="30" max="30" width="63.85546875" customWidth="1"/>
     <col min="31" max="31" width="59.42578125" customWidth="1"/>
@@ -937,7 +939,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -952,10 +954,10 @@
         <v>53</v>
       </c>
       <c r="F1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" t="s">
         <v>165</v>
-      </c>
-      <c r="G1" t="s">
-        <v>166</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -985,64 +987,64 @@
         <v>39</v>
       </c>
       <c r="Q1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R1" t="s">
         <v>131</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>132</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>133</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>134</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>135</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>136</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>137</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>138</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI1" t="s">
         <v>141</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>143</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1065,7 +1067,7 @@
         <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K2" t="s">
         <v>12</v>
@@ -1074,7 +1076,7 @@
         <v>33</v>
       </c>
       <c r="AB2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC2" t="s">
         <v>40</v>
@@ -1115,7 +1117,7 @@
         <v>33</v>
       </c>
       <c r="AB3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC3" t="s">
         <v>43</v>
@@ -1147,7 +1149,7 @@
         <v>31</v>
       </c>
       <c r="AB4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC4" t="s">
         <v>44</v>
@@ -1188,7 +1190,7 @@
         <v>103</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K5" t="s">
         <v>12</v>
@@ -1200,7 +1202,7 @@
         <v>30</v>
       </c>
       <c r="AB5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC5" t="s">
         <v>45</v>
@@ -1211,7 +1213,7 @@
         <v>1012</v>
       </c>
       <c r="B6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
@@ -1232,7 +1234,7 @@
         <v>31</v>
       </c>
       <c r="AB6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC6" t="s">
         <v>45</v>
@@ -1243,7 +1245,7 @@
         <v>1013</v>
       </c>
       <c r="B7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
@@ -1264,7 +1266,7 @@
         <v>30</v>
       </c>
       <c r="AB7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC7" t="s">
         <v>43</v>
@@ -1275,7 +1277,7 @@
         <v>1014</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
@@ -1296,7 +1298,7 @@
         <v>30</v>
       </c>
       <c r="AB8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC8" t="s">
         <v>43</v>
@@ -1307,7 +1309,7 @@
         <v>1015</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -1328,7 +1330,7 @@
         <v>33</v>
       </c>
       <c r="AB9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC9" t="s">
         <v>47</v>
@@ -1339,7 +1341,7 @@
         <v>1016</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
@@ -1360,7 +1362,7 @@
         <v>32</v>
       </c>
       <c r="AB10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC10" t="s">
         <v>45</v>
@@ -1371,7 +1373,7 @@
         <v>1017</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
@@ -1392,7 +1394,7 @@
         <v>34</v>
       </c>
       <c r="AB11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC11" t="s">
         <v>47</v>
@@ -1403,7 +1405,7 @@
         <v>1018</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
@@ -1424,7 +1426,7 @@
         <v>30</v>
       </c>
       <c r="AB12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC12" t="s">
         <v>43</v>
@@ -1435,25 +1437,25 @@
         <v>549</v>
       </c>
       <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="D13" t="s">
         <v>161</v>
-      </c>
-      <c r="D13" t="s">
-        <v>162</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L13" t="s">
         <v>31</v>
       </c>
       <c r="AB13" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC13" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1483,8 +1485,8 @@
   <dimension ref="A1:AJ11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G18" sqref="G18"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1498,6 +1500,7 @@
     <col min="7" max="7" width="20.7109375" customWidth="1"/>
     <col min="8" max="8" width="19.85546875" customWidth="1"/>
     <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="27" max="27" width="9.140625" style="1"/>
     <col min="29" max="29" width="71.85546875" customWidth="1"/>
     <col min="30" max="30" width="63.85546875" customWidth="1"/>
     <col min="31" max="31" width="59.42578125" customWidth="1"/>
@@ -1508,7 +1511,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1523,10 +1526,10 @@
         <v>53</v>
       </c>
       <c r="F1" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" t="s">
         <v>165</v>
-      </c>
-      <c r="G1" t="s">
-        <v>166</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1556,64 +1559,64 @@
         <v>39</v>
       </c>
       <c r="Q1" t="s">
+        <v>130</v>
+      </c>
+      <c r="R1" t="s">
         <v>131</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>132</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>133</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>134</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>135</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>136</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>137</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>138</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>139</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>140</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>114</v>
+      </c>
+      <c r="AI1" t="s">
         <v>141</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>143</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>115</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1633,7 +1636,7 @@
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -1641,8 +1644,11 @@
       <c r="L2" t="s">
         <v>32</v>
       </c>
+      <c r="AA2" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="AB2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC2" t="s">
         <v>41</v>
@@ -1674,10 +1680,10 @@
         <v>102</v>
       </c>
       <c r="G3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="K3" t="s">
         <v>13</v>
@@ -1685,8 +1691,11 @@
       <c r="L3" t="s">
         <v>31</v>
       </c>
+      <c r="AA3" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="AB3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC3" t="s">
         <v>42</v>
@@ -1709,7 +1718,7 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
@@ -1718,7 +1727,7 @@
         <v>34</v>
       </c>
       <c r="AB4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC4" t="s">
         <v>46</v>
@@ -1744,10 +1753,10 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
@@ -1755,8 +1764,11 @@
       <c r="L5" t="s">
         <v>34</v>
       </c>
+      <c r="AA5" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="AB5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC5" t="s">
         <v>47</v>
@@ -1767,16 +1779,16 @@
         <v>205</v>
       </c>
       <c r="B6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" t="s">
         <v>147</v>
-      </c>
-      <c r="D6" t="s">
-        <v>148</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
@@ -1785,10 +1797,10 @@
         <v>32</v>
       </c>
       <c r="AB6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -1796,16 +1808,16 @@
         <v>205</v>
       </c>
       <c r="B7" t="s">
+        <v>146</v>
+      </c>
+      <c r="D7" t="s">
         <v>147</v>
-      </c>
-      <c r="D7" t="s">
-        <v>148</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K7" t="s">
         <v>13</v>
@@ -1813,11 +1825,14 @@
       <c r="L7" t="s">
         <v>32</v>
       </c>
+      <c r="AA7" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="AB7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -1825,16 +1840,16 @@
         <v>205</v>
       </c>
       <c r="B8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D8" t="s">
         <v>147</v>
-      </c>
-      <c r="D8" t="s">
-        <v>148</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K8" t="s">
         <v>13</v>
@@ -1842,11 +1857,14 @@
       <c r="L8" t="s">
         <v>32</v>
       </c>
+      <c r="AA8" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="AB8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -1854,16 +1872,16 @@
         <v>205</v>
       </c>
       <c r="B9" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" t="s">
         <v>147</v>
-      </c>
-      <c r="D9" t="s">
-        <v>148</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K9" t="s">
         <v>13</v>
@@ -1871,11 +1889,14 @@
       <c r="L9" t="s">
         <v>32</v>
       </c>
+      <c r="AA9" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="AB9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -1883,16 +1904,16 @@
         <v>205</v>
       </c>
       <c r="B10" t="s">
+        <v>146</v>
+      </c>
+      <c r="D10" t="s">
         <v>147</v>
-      </c>
-      <c r="D10" t="s">
-        <v>148</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K10" t="s">
         <v>13</v>
@@ -1900,11 +1921,14 @@
       <c r="L10" t="s">
         <v>32</v>
       </c>
+      <c r="AA10" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="AB10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AC10" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -1912,25 +1936,28 @@
         <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L11" t="s">
         <v>32</v>
       </c>
+      <c r="AA11" s="1" t="s">
+        <v>166</v>
+      </c>
       <c r="AB11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AC11" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2020,7 +2047,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2028,7 +2055,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -2688,7 +2715,7 @@
         <v>69</v>
       </c>
       <c r="B53" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
@@ -2700,7 +2727,7 @@
         <v>70</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -2712,7 +2739,7 @@
         <v>71</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -2724,7 +2751,7 @@
         <v>72</v>
       </c>
       <c r="B56" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -2736,7 +2763,7 @@
         <v>73</v>
       </c>
       <c r="B57" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
@@ -2748,7 +2775,7 @@
         <v>74</v>
       </c>
       <c r="B58" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -2760,7 +2787,7 @@
         <v>75</v>
       </c>
       <c r="B59" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -2772,7 +2799,7 @@
         <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -2784,7 +2811,7 @@
         <v>77</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
@@ -2796,7 +2823,7 @@
         <v>78</v>
       </c>
       <c r="B62" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
@@ -2808,7 +2835,7 @@
         <v>79</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
@@ -2820,7 +2847,7 @@
         <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
@@ -2832,7 +2859,7 @@
         <v>81</v>
       </c>
       <c r="B65" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
@@ -2844,7 +2871,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
@@ -2856,7 +2883,7 @@
         <v>82</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="1"/>
@@ -2868,7 +2895,7 @@
         <v>83</v>
       </c>
       <c r="B68" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -2880,7 +2907,7 @@
         <v>84</v>
       </c>
       <c r="B69" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -2892,7 +2919,7 @@
         <v>85</v>
       </c>
       <c r="B70" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -2904,7 +2931,7 @@
         <v>86</v>
       </c>
       <c r="B71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -2916,7 +2943,7 @@
         <v>87</v>
       </c>
       <c r="B72" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -2928,7 +2955,7 @@
         <v>88</v>
       </c>
       <c r="B73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -2940,7 +2967,7 @@
         <v>89</v>
       </c>
       <c r="B74" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -2952,7 +2979,7 @@
         <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -2964,7 +2991,7 @@
         <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -2976,7 +3003,7 @@
         <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -2988,7 +3015,7 @@
         <v>92</v>
       </c>
       <c r="B78" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -3000,7 +3027,7 @@
         <v>93</v>
       </c>
       <c r="B79" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -3012,7 +3039,7 @@
         <v>94</v>
       </c>
       <c r="B80" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
@@ -3024,7 +3051,7 @@
         <v>95</v>
       </c>
       <c r="B81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
@@ -3036,7 +3063,7 @@
         <v>96</v>
       </c>
       <c r="B82" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
@@ -3048,7 +3075,7 @@
         <v>97</v>
       </c>
       <c r="B83" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
@@ -3057,10 +3084,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B84" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
@@ -3069,10 +3096,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B85" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
@@ -3081,10 +3108,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -3093,10 +3120,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B87" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -3125,17 +3152,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3165,7 +3192,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -3240,7 +3267,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add fetchable selection of colors
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C498D89C-D650-4631-AB54-4D8303A7EB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B12B69-3422-4C94-BC88-61296DC15A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
     <sheet name="Embroidery Designs" sheetId="1" r:id="rId2"/>
-    <sheet name="Categories" sheetId="2" r:id="rId3"/>
-    <sheet name="Subcategories" sheetId="3" r:id="rId4"/>
-    <sheet name="Status" sheetId="8" r:id="rId5"/>
-    <sheet name="YesNo" sheetId="4" r:id="rId6"/>
-    <sheet name="Tags" sheetId="5" r:id="rId7"/>
-    <sheet name="DesignType" sheetId="6" r:id="rId8"/>
+    <sheet name="Colors" sheetId="9" r:id="rId3"/>
+    <sheet name="Categories" sheetId="2" r:id="rId4"/>
+    <sheet name="Subcategories" sheetId="3" r:id="rId5"/>
+    <sheet name="Status" sheetId="8" r:id="rId6"/>
+    <sheet name="YesNo" sheetId="4" r:id="rId7"/>
+    <sheet name="Tags" sheetId="5" r:id="rId8"/>
+    <sheet name="DesignType" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="Categories">Categories!$A$2:$A$1048576</definedName>
+    <definedName name="Colors">Colors!$A:$A</definedName>
     <definedName name="DesignType">DesignType!$A$1:$A$2</definedName>
     <definedName name="Status">Status!$A$1:$A$2</definedName>
     <definedName name="Subcategories">Subcategories!$C$2:$C$1048576</definedName>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="187">
   <si>
     <t>Name</t>
   </si>
@@ -131,15 +133,6 @@
     <t>Cras fermentum odio eu feugiat. Risus quis varius quam quisque. Duis at tellus at urna condimentum mattis pellentesque id nibh.</t>
   </si>
   <si>
-    <t>#556271</t>
-  </si>
-  <si>
-    <t>#ff6a67</t>
-  </si>
-  <si>
-    <t>#f4f6f8</t>
-  </si>
-  <si>
     <t>Hierarchy</t>
   </si>
   <si>
@@ -494,9 +487,6 @@
     <t>Union Swirl</t>
   </si>
   <si>
-    <t>#000000</t>
-  </si>
-  <si>
     <t>Union Specific &gt; IAM</t>
   </si>
   <si>
@@ -536,9 +526,6 @@
     <t>Oversize Design</t>
   </si>
   <si>
-    <t>#000001</t>
-  </si>
-  <si>
     <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/549 (Oversize).jpg</t>
   </si>
   <si>
@@ -552,13 +539,88 @@
   </si>
   <si>
     <t>1/1/2024</t>
+  </si>
+  <si>
+    <t>#F2F3EF - White</t>
+  </si>
+  <si>
+    <t>#282627 - Black</t>
+  </si>
+  <si>
+    <t>#CB6138 - Bright Orange</t>
+  </si>
+  <si>
+    <t>#8C4744 - Cardinal</t>
+  </si>
+  <si>
+    <t>#706F74 - Charcoal</t>
+  </si>
+  <si>
+    <t>#393130 - Chocolate</t>
+  </si>
+  <si>
+    <t>#888A90 - Dark Ash</t>
+  </si>
+  <si>
+    <t>#292B31 - Dark Navy</t>
+  </si>
+  <si>
+    <t>#E8B061 - Gold</t>
+  </si>
+  <si>
+    <t>#314D3E - Hunter Green</t>
+  </si>
+  <si>
+    <t>#649F66 - Irish Kelly</t>
+  </si>
+  <si>
+    <t>#A9BBC7 - Light Blue</t>
+  </si>
+  <si>
+    <t>#DFE074 - Lime Green</t>
+  </si>
+  <si>
+    <t>#ECE6E4 - Natural</t>
+  </si>
+  <si>
+    <t>#0c1933 - Navy</t>
+  </si>
+  <si>
+    <t>#605D4E - Olive</t>
+  </si>
+  <si>
+    <t>#E7C2CB - Pink</t>
+  </si>
+  <si>
+    <t>#46326f - Purple</t>
+  </si>
+  <si>
+    <t>#A33434 - Red</t>
+  </si>
+  <si>
+    <t>#335491 - Royal</t>
+  </si>
+  <si>
+    <t>#D6C880 - Yellow</t>
+  </si>
+  <si>
+    <t>#b2ff00 - Safety Green</t>
+  </si>
+  <si>
+    <t>#383838 - Charcoal Heather</t>
+  </si>
+  <si>
+    <t>#d19e6c - Sand</t>
+  </si>
+  <si>
+    <t>Color</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,6 +630,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -593,9 +662,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -913,8 +983,8 @@
   <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA2" sqref="AA2:AA1048576"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D2" sqref="D2:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,7 +1009,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -951,13 +1021,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -969,82 +1039,82 @@
         <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" t="s">
-        <v>39</v>
-      </c>
       <c r="Q1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" t="s">
         <v>130</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>131</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>132</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>133</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>134</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>135</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>136</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>137</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI1" t="s">
         <v>138</v>
       </c>
-      <c r="Z1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AJ1" t="s">
         <v>140</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1058,31 +1128,31 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>167</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K2" t="s">
         <v>12</v>
       </c>
       <c r="L2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AB2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="AD2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1096,31 +1166,31 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
       </c>
       <c r="L3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N3" t="s">
-        <v>33</v>
-      </c>
       <c r="AB3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
@@ -1134,40 +1204,40 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AB4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH4" t="s">
         <v>44</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>46</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -1181,31 +1251,31 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>171</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K5" t="s">
         <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="M5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AB5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -1213,31 +1283,31 @@
         <v>1012</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K6" t="s">
         <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AB6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -1245,31 +1315,31 @@
         <v>1013</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K7" t="s">
         <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AB7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -1277,31 +1347,31 @@
         <v>1014</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>164</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K8" t="s">
         <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AB8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -1309,31 +1379,31 @@
         <v>1015</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>180</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K9" t="s">
         <v>12</v>
       </c>
       <c r="L9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="AB9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -1341,31 +1411,31 @@
         <v>1016</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>166</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K10" t="s">
         <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AB10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -1373,31 +1443,31 @@
         <v>1017</v>
       </c>
       <c r="B11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>177</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K11" t="s">
         <v>12</v>
       </c>
       <c r="L11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AB11" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC11" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
@@ -1405,31 +1475,31 @@
         <v>1018</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>168</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="K12" t="s">
         <v>12</v>
       </c>
       <c r="L12" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="AB12" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
@@ -1437,29 +1507,29 @@
         <v>549</v>
       </c>
       <c r="B13" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D13" t="s">
-        <v>161</v>
+        <v>169</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="L13" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AB13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC13" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{A61431EB-F298-41CC-8A14-D29D28DE34A1}">
       <formula1>DesignType</formula1>
     </dataValidation>
@@ -1475,6 +1545,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1048576" xr:uid="{99999286-3ED4-4B5C-B2BF-6EDC933F7B52}">
       <formula1>Status</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{89425058-0C05-4809-93A2-EBBE8CA5B4F6}">
+      <formula1>Colors</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1484,9 +1557,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
   <dimension ref="A1:AJ11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1511,7 +1584,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1523,13 +1596,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="G1" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1541,82 +1614,82 @@
         <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="L1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" t="s">
         <v>35</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" t="s">
-        <v>39</v>
-      </c>
       <c r="Q1" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1" t="s">
+        <v>128</v>
+      </c>
+      <c r="S1" t="s">
+        <v>129</v>
+      </c>
+      <c r="T1" t="s">
         <v>130</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>131</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>132</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>133</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>134</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>135</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>136</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>137</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AI1" t="s">
         <v>138</v>
       </c>
-      <c r="Z1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AJ1" t="s">
         <v>140</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>112</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>113</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>114</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1630,34 +1703,34 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>167</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
       </c>
       <c r="L2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="AD2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="AE2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1671,34 +1744,34 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>164</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G3" t="s">
         <v>102</v>
       </c>
-      <c r="G3" t="s">
-        <v>105</v>
-      </c>
       <c r="H3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="K3" t="s">
         <v>13</v>
       </c>
       <c r="L3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
@@ -1712,28 +1785,28 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>170</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AB4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AD4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -1747,31 +1820,31 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>171</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
       </c>
       <c r="L5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -1779,28 +1852,28 @@
         <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
       </c>
       <c r="L6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AB6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC6" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -1808,31 +1881,31 @@
         <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="K7" t="s">
         <v>13</v>
       </c>
       <c r="L7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -1840,31 +1913,31 @@
         <v>205</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="K8" t="s">
         <v>13</v>
       </c>
       <c r="L8" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB8" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -1872,31 +1945,31 @@
         <v>205</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>180</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="K9" t="s">
         <v>13</v>
       </c>
       <c r="L9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC9" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -1904,31 +1977,31 @@
         <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>166</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="K10" t="s">
         <v>13</v>
       </c>
       <c r="L10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB10" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="AC10" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -1936,33 +2009,33 @@
         <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="L11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="AB11" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="AC11" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11 E13:E1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
       <formula1>YesNo</formula1>
     </dataValidation>
@@ -1978,6 +2051,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB11 AB13:AB1048576" xr:uid="{9EF19CFE-4BEB-4B6E-9893-F1BFEBCAA2B4}">
       <formula1>Status</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{510EF69A-8273-4570-9E7F-349E731D2D60}">
+      <formula1>Colors</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1985,6 +2061,149 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F0CF4C-AC02-46A4-BD1F-193963CE75CB}">
+  <dimension ref="A1:A25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE8B92B-2F2F-44F6-BB2D-490F7DE9352F}">
   <dimension ref="A1:B8"/>
   <sheetViews>
@@ -2002,12 +2221,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -2015,7 +2234,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2031,7 +2250,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -2039,7 +2258,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -2047,7 +2266,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2055,7 +2274,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -2072,7 +2291,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1586536D-3214-4B71-B711-EFBAF2410143}">
   <dimension ref="A1:C87"/>
   <sheetViews>
@@ -2095,15 +2314,15 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C33" si="0">_xlfn.CONCAT(B2, " &gt; ", A2)</f>
@@ -2112,10 +2331,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -2124,10 +2343,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -2136,10 +2355,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -2148,10 +2367,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -2160,10 +2379,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -2172,10 +2391,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2184,10 +2403,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -2196,10 +2415,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -2208,10 +2427,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B11" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -2220,10 +2439,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2232,10 +2451,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -2244,10 +2463,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -2268,7 +2487,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -2280,7 +2499,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -2292,10 +2511,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -2304,10 +2523,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -2316,10 +2535,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -2328,10 +2547,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -2340,10 +2559,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -2352,10 +2571,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -2364,10 +2583,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -2376,10 +2595,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -2388,10 +2607,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -2400,10 +2619,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -2412,10 +2631,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -2424,10 +2643,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -2436,10 +2655,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -2448,10 +2667,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -2463,7 +2682,7 @@
         <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -2472,10 +2691,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -2484,10 +2703,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" ref="C34:C87" si="1">_xlfn.CONCAT(B34, " &gt; ", A34)</f>
@@ -2496,10 +2715,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
@@ -2508,10 +2727,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
@@ -2520,10 +2739,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
@@ -2532,10 +2751,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B38" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
@@ -2544,10 +2763,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B39" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
@@ -2556,10 +2775,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B40" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
@@ -2568,10 +2787,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
@@ -2580,10 +2799,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B42" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
@@ -2595,7 +2814,7 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
@@ -2604,10 +2823,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
@@ -2616,10 +2835,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B45" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
@@ -2628,10 +2847,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
@@ -2640,10 +2859,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B47" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
@@ -2652,10 +2871,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
@@ -2664,10 +2883,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
@@ -2676,10 +2895,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
@@ -2688,10 +2907,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
@@ -2700,10 +2919,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
@@ -2712,10 +2931,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B53" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
@@ -2724,10 +2943,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B54" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -2736,10 +2955,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B55" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -2748,10 +2967,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B56" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -2760,10 +2979,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B57" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
@@ -2772,10 +2991,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B58" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -2784,10 +3003,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -2796,10 +3015,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -2808,10 +3027,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B61" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
@@ -2820,10 +3039,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B62" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
@@ -2832,10 +3051,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B63" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
@@ -2844,10 +3063,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B64" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
@@ -2856,10 +3075,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
@@ -2871,7 +3090,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
@@ -2880,10 +3099,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B67" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="1"/>
@@ -2892,10 +3111,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B68" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -2904,10 +3123,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B69" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -2916,10 +3135,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B70" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -2928,10 +3147,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B71" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -2940,10 +3159,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -2952,10 +3171,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -2964,10 +3183,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B74" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -2976,10 +3195,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B75" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -2988,10 +3207,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B76" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -3003,7 +3222,7 @@
         <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -3012,10 +3231,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B78" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -3024,10 +3243,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B79" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -3036,10 +3255,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B80" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
@@ -3048,10 +3267,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B81" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
@@ -3060,10 +3279,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B82" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
@@ -3072,10 +3291,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B83" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
@@ -3084,10 +3303,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B84" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
@@ -3096,10 +3315,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B85" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
@@ -3108,10 +3327,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B86" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -3120,10 +3339,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B87" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -3140,7 +3359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8207F966-3498-4646-82AC-E7F049D20E38}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3152,17 +3371,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3170,7 +3389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBDC08E-FD24-497A-86A5-D3DBD82D6691}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3192,7 +3411,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -3200,7 +3419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{096F644A-6816-46A6-9C37-F543D22E3BF1}">
   <dimension ref="A1:A6"/>
   <sheetViews>
@@ -3217,27 +3436,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -3245,7 +3464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77A83CC9-1574-4180-85AD-01F92A9D1604}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3267,7 +3486,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix design age classification; add tests to validate
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B12B69-3422-4C94-BC88-61296DC15A3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C48570-1CEB-4CB8-9981-31B05C7D9AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="189">
   <si>
     <t>Name</t>
   </si>
@@ -614,6 +614,12 @@
   </si>
   <si>
     <t>Color</t>
+  </si>
+  <si>
+    <t>1/1/2017</t>
+  </si>
+  <si>
+    <t>Quick Search &gt; Patriotic</t>
   </si>
 </sst>
 </file>
@@ -982,9 +988,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
   <dimension ref="A1:AJ13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D2" sqref="D2:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F6" sqref="F6:F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,6 +1151,9 @@
       <c r="L2" t="s">
         <v>30</v>
       </c>
+      <c r="AA2" s="1" t="s">
+        <v>187</v>
+      </c>
       <c r="AB2" t="s">
         <v>141</v>
       </c>
@@ -1172,7 +1181,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -1185,6 +1194,9 @@
       </c>
       <c r="N3" t="s">
         <v>30</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="AB3" t="s">
         <v>141</v>
@@ -1210,13 +1222,16 @@
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
       </c>
       <c r="L4" t="s">
         <v>28</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="AB4" t="s">
         <v>141</v>
@@ -1271,6 +1286,9 @@
       <c r="M5" t="s">
         <v>27</v>
       </c>
+      <c r="AA5" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="AB5" t="s">
         <v>141</v>
       </c>
@@ -1295,13 +1313,16 @@
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K6" t="s">
         <v>12</v>
       </c>
       <c r="L6" t="s">
         <v>28</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="AB6" t="s">
         <v>141</v>
@@ -1327,13 +1348,16 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K7" t="s">
         <v>12</v>
       </c>
       <c r="L7" t="s">
         <v>27</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="AB7" t="s">
         <v>141</v>
@@ -1359,13 +1383,16 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K8" t="s">
         <v>12</v>
       </c>
       <c r="L8" t="s">
         <v>27</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="AB8" t="s">
         <v>141</v>
@@ -1391,13 +1418,16 @@
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K9" t="s">
         <v>12</v>
       </c>
       <c r="L9" t="s">
         <v>30</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="AB9" t="s">
         <v>141</v>
@@ -1423,13 +1453,16 @@
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K10" t="s">
         <v>12</v>
       </c>
       <c r="L10" t="s">
         <v>29</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="AB10" t="s">
         <v>141</v>
@@ -1455,13 +1488,16 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K11" t="s">
         <v>12</v>
       </c>
       <c r="L11" t="s">
         <v>31</v>
+      </c>
+      <c r="AA11" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="AB11" t="s">
         <v>141</v>
@@ -1487,13 +1523,16 @@
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>188</v>
       </c>
       <c r="K12" t="s">
         <v>12</v>
       </c>
       <c r="L12" t="s">
         <v>27</v>
+      </c>
+      <c r="AA12" s="1" t="s">
+        <v>187</v>
       </c>
       <c r="AB12" t="s">
         <v>141</v>
@@ -1521,6 +1560,9 @@
       <c r="L13" t="s">
         <v>28</v>
       </c>
+      <c r="AA13" s="1" t="s">
+        <v>161</v>
+      </c>
       <c r="AB13" t="s">
         <v>141</v>
       </c>
@@ -1529,6 +1571,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{A61431EB-F298-41CC-8A14-D29D28DE34A1}">
       <formula1>DesignType</formula1>
@@ -1558,8 +1601,8 @@
   <dimension ref="A1:AJ11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D9" sqref="D9"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41F0CF4C-AC02-46A4-BD1F-193963CE75CB}">
   <dimension ref="A1:A25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add basic image transparency detection
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25C48570-1CEB-4CB8-9981-31B05C7D9AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC305E93-0998-445C-B100-583BCFC4DF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -178,9 +178,6 @@
     <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1648.jpg</t>
   </si>
   <si>
-    <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1649.jpg</t>
-  </si>
-  <si>
     <t>/IP Design Library/IP New Designs_2023 Spring-Summer/1650.jpg</t>
   </si>
   <si>
@@ -620,6 +617,9 @@
   </si>
   <si>
     <t>Quick Search &gt; Patriotic</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Design Library-PNGs (1200px)/910-darks.png</t>
   </si>
 </sst>
 </file>
@@ -989,8 +989,8 @@
   <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F6" sqref="F6:F12"/>
+      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +1015,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1027,13 +1027,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
         <v>159</v>
-      </c>
-      <c r="G1" t="s">
-        <v>160</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1045,7 +1045,7 @@
         <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L1" t="s">
         <v>32</v>
@@ -1063,64 +1063,64 @@
         <v>36</v>
       </c>
       <c r="Q1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" t="s">
         <v>127</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>128</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>129</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>130</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>131</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>132</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>133</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>134</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>135</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI1" t="s">
         <v>137</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>139</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1134,16 +1134,16 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K2" t="s">
         <v>12</v>
@@ -1152,10 +1152,10 @@
         <v>30</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC2" t="s">
         <v>37</v>
@@ -1175,13 +1175,13 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -1196,10 +1196,10 @@
         <v>30</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC3" t="s">
         <v>40</v>
@@ -1216,13 +1216,13 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
@@ -1231,13 +1231,13 @@
         <v>28</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC4" t="s">
-        <v>41</v>
+        <v>188</v>
       </c>
       <c r="AD4" t="s">
         <v>39</v>
@@ -1246,13 +1246,13 @@
         <v>38</v>
       </c>
       <c r="AF4" t="s">
+        <v>42</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH4" t="s">
         <v>43</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
@@ -1266,16 +1266,16 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K5" t="s">
         <v>12</v>
@@ -1287,13 +1287,13 @@
         <v>27</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -1301,19 +1301,19 @@
         <v>1012</v>
       </c>
       <c r="B6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K6" t="s">
         <v>12</v>
@@ -1322,13 +1322,13 @@
         <v>28</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -1336,19 +1336,19 @@
         <v>1013</v>
       </c>
       <c r="B7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K7" t="s">
         <v>12</v>
@@ -1357,10 +1357,10 @@
         <v>27</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC7" t="s">
         <v>40</v>
@@ -1371,19 +1371,19 @@
         <v>1014</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K8" t="s">
         <v>12</v>
@@ -1392,10 +1392,10 @@
         <v>27</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC8" t="s">
         <v>40</v>
@@ -1406,19 +1406,19 @@
         <v>1015</v>
       </c>
       <c r="B9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K9" t="s">
         <v>12</v>
@@ -1427,13 +1427,13 @@
         <v>30</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -1441,19 +1441,19 @@
         <v>1016</v>
       </c>
       <c r="B10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K10" t="s">
         <v>12</v>
@@ -1462,13 +1462,13 @@
         <v>29</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -1476,19 +1476,19 @@
         <v>1017</v>
       </c>
       <c r="B11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K11" t="s">
         <v>12</v>
@@ -1497,13 +1497,13 @@
         <v>31</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
@@ -1511,19 +1511,19 @@
         <v>1018</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="K12" t="s">
         <v>12</v>
@@ -1532,10 +1532,10 @@
         <v>27</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AB12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC12" t="s">
         <v>40</v>
@@ -1546,28 +1546,28 @@
         <v>549</v>
       </c>
       <c r="B13" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="L13" t="s">
         <v>28</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC13" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1627,7 +1627,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1639,13 +1639,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G1" t="s">
         <v>159</v>
-      </c>
-      <c r="G1" t="s">
-        <v>160</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1657,7 +1657,7 @@
         <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L1" t="s">
         <v>32</v>
@@ -1675,64 +1675,64 @@
         <v>36</v>
       </c>
       <c r="Q1" t="s">
+        <v>126</v>
+      </c>
+      <c r="R1" t="s">
         <v>127</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>128</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>129</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>130</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>131</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>132</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>133</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>134</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>135</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>136</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>107</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>110</v>
+      </c>
+      <c r="AI1" t="s">
         <v>137</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>139</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>111</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -1746,13 +1746,13 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -1761,10 +1761,10 @@
         <v>29</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC2" t="s">
         <v>38</v>
@@ -1773,7 +1773,7 @@
         <v>39</v>
       </c>
       <c r="AE2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -1787,19 +1787,19 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K3" t="s">
         <v>13</v>
@@ -1808,10 +1808,10 @@
         <v>28</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC3" t="s">
         <v>39</v>
@@ -1828,13 +1828,13 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
@@ -1843,10 +1843,10 @@
         <v>31</v>
       </c>
       <c r="AB4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AD4" t="s">
         <v>39</v>
@@ -1863,16 +1863,16 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
@@ -1881,13 +1881,13 @@
         <v>31</v>
       </c>
       <c r="AA5" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -1895,16 +1895,16 @@
         <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
@@ -1913,10 +1913,10 @@
         <v>29</v>
       </c>
       <c r="AB6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">
@@ -1924,16 +1924,16 @@
         <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K7" t="s">
         <v>13</v>
@@ -1942,13 +1942,13 @@
         <v>29</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:36" x14ac:dyDescent="0.25">
@@ -1956,16 +1956,16 @@
         <v>205</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K8" t="s">
         <v>13</v>
@@ -1974,13 +1974,13 @@
         <v>29</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.25">
@@ -1988,16 +1988,16 @@
         <v>205</v>
       </c>
       <c r="B9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="K9" t="s">
         <v>13</v>
@@ -2006,13 +2006,13 @@
         <v>29</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:36" x14ac:dyDescent="0.25">
@@ -2020,16 +2020,16 @@
         <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="K10" t="s">
         <v>13</v>
@@ -2038,13 +2038,13 @@
         <v>29</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AC10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
@@ -2052,28 +2052,28 @@
         <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D11" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L11" t="s">
         <v>29</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AB11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="AC11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -2118,127 +2118,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2264,12 +2264,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" t="s">
         <v>12</v>
@@ -2293,7 +2293,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -2301,7 +2301,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -2309,7 +2309,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2317,7 +2317,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -2362,10 +2362,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C33" si="0">_xlfn.CONCAT(B2, " &gt; ", A2)</f>
@@ -2374,10 +2374,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
@@ -2386,10 +2386,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -2398,10 +2398,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -2413,7 +2413,7 @@
         <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -2422,10 +2422,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -2434,10 +2434,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -2446,10 +2446,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -2458,10 +2458,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -2470,10 +2470,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -2482,10 +2482,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2494,10 +2494,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
@@ -2506,10 +2506,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -2530,7 +2530,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" t="s">
         <v>3</v>
@@ -2542,7 +2542,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -2554,10 +2554,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -2566,10 +2566,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -2578,10 +2578,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
@@ -2590,10 +2590,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -2602,10 +2602,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -2614,10 +2614,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -2626,10 +2626,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
@@ -2638,10 +2638,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -2650,10 +2650,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
@@ -2662,10 +2662,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
@@ -2674,10 +2674,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
@@ -2686,10 +2686,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
@@ -2698,10 +2698,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
@@ -2710,10 +2710,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
@@ -2725,7 +2725,7 @@
         <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="0"/>
@@ -2734,10 +2734,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="0"/>
@@ -2746,10 +2746,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" ref="C34:C87" si="1">_xlfn.CONCAT(B34, " &gt; ", A34)</f>
@@ -2758,10 +2758,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B35" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
@@ -2770,10 +2770,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
@@ -2782,10 +2782,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
@@ -2794,10 +2794,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
@@ -2806,10 +2806,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
@@ -2818,10 +2818,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
@@ -2830,10 +2830,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
@@ -2842,10 +2842,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
@@ -2857,7 +2857,7 @@
         <v>16</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
@@ -2866,10 +2866,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C44" t="str">
         <f t="shared" si="1"/>
@@ -2878,10 +2878,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C45" t="str">
         <f t="shared" si="1"/>
@@ -2890,10 +2890,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C46" t="str">
         <f t="shared" si="1"/>
@@ -2902,10 +2902,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C47" t="str">
         <f t="shared" si="1"/>
@@ -2914,10 +2914,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" t="str">
         <f t="shared" si="1"/>
@@ -2926,10 +2926,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="1"/>
@@ -2938,10 +2938,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="1"/>
@@ -2950,10 +2950,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="1"/>
@@ -2962,10 +2962,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" t="str">
         <f t="shared" si="1"/>
@@ -2974,10 +2974,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
@@ -2986,10 +2986,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -2998,10 +2998,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -3010,10 +3010,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -3022,10 +3022,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
@@ -3034,10 +3034,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -3046,10 +3046,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -3058,10 +3058,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -3070,10 +3070,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
@@ -3082,10 +3082,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
@@ -3094,10 +3094,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
@@ -3106,10 +3106,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
@@ -3118,10 +3118,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
@@ -3133,7 +3133,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
@@ -3142,10 +3142,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="1"/>
@@ -3154,10 +3154,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -3166,10 +3166,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -3178,10 +3178,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -3190,10 +3190,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -3202,10 +3202,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B72" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -3214,10 +3214,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -3226,10 +3226,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B74" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -3238,10 +3238,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -3250,10 +3250,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -3265,7 +3265,7 @@
         <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -3274,10 +3274,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B78" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -3286,10 +3286,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -3298,10 +3298,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
@@ -3310,10 +3310,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
@@ -3322,10 +3322,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
@@ -3334,10 +3334,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
@@ -3346,10 +3346,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B84" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
@@ -3358,10 +3358,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B85" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
@@ -3370,10 +3370,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B86" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -3382,10 +3382,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B87" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -3414,17 +3414,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3454,7 +3454,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -3529,7 +3529,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add optional priority to designs and option to sort by it
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC305E93-0998-445C-B100-583BCFC4DF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E0348B-E86F-456C-AED8-026109A6775B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="190">
   <si>
     <t>Name</t>
   </si>
@@ -620,6 +620,9 @@
   </si>
   <si>
     <t>/Marketing/Website/Design Library/Design Library-PNGs (1200px)/910-darks.png</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -986,34 +989,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
-  <dimension ref="A1:AJ13"/>
+  <dimension ref="A1:AK13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="V1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AC4" sqref="AC4"/>
+      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA12" sqref="AA12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="90.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="29.5703125" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" style="1"/>
-    <col min="29" max="29" width="71.85546875" customWidth="1"/>
-    <col min="30" max="30" width="63.85546875" customWidth="1"/>
-    <col min="31" max="31" width="59.42578125" customWidth="1"/>
-    <col min="32" max="32" width="60.140625" customWidth="1"/>
-    <col min="33" max="33" width="61.42578125" customWidth="1"/>
-    <col min="34" max="34" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="90.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1"/>
+    <col min="6" max="6" width="27.44140625" customWidth="1"/>
+    <col min="7" max="7" width="29.5546875" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="28" max="28" width="9.109375" style="1"/>
+    <col min="30" max="30" width="71.88671875" customWidth="1"/>
+    <col min="31" max="31" width="63.88671875" customWidth="1"/>
+    <col min="32" max="32" width="59.44140625" customWidth="1"/>
+    <col min="33" max="33" width="60.109375" customWidth="1"/>
+    <col min="34" max="34" width="61.44140625" customWidth="1"/>
+    <col min="35" max="35" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1093,37 +1096,40 @@
         <v>135</v>
       </c>
       <c r="AA1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB1" t="s">
         <v>136</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>138</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>105</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>107</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>106</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>108</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>109</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>110</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>137</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1025</v>
       </c>
@@ -1151,20 +1157,23 @@
       <c r="L2" t="s">
         <v>30</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>140</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>37</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1003</v>
       </c>
@@ -1195,17 +1204,17 @@
       <c r="N3" t="s">
         <v>30</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AB3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>140</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1230,32 +1239,32 @@
       <c r="L4" t="s">
         <v>28</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>140</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>188</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>39</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>38</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>42</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>41</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1286,17 +1295,17 @@
       <c r="M5" t="s">
         <v>27</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>140</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1012</v>
       </c>
@@ -1321,17 +1330,20 @@
       <c r="L6" t="s">
         <v>28</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AA6">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>140</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1013</v>
       </c>
@@ -1356,17 +1368,17 @@
       <c r="L7" t="s">
         <v>27</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>140</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1014</v>
       </c>
@@ -1391,17 +1403,17 @@
       <c r="L8" t="s">
         <v>27</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>140</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1015</v>
       </c>
@@ -1426,17 +1438,17 @@
       <c r="L9" t="s">
         <v>30</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>140</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1016</v>
       </c>
@@ -1461,17 +1473,20 @@
       <c r="L10" t="s">
         <v>29</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AA10">
+        <v>2</v>
+      </c>
+      <c r="AB10" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>140</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1017</v>
       </c>
@@ -1496,17 +1511,17 @@
       <c r="L11" t="s">
         <v>31</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>140</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1018</v>
       </c>
@@ -1531,17 +1546,17 @@
       <c r="L12" t="s">
         <v>27</v>
       </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AB12" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>140</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>549</v>
       </c>
@@ -1560,13 +1575,13 @@
       <c r="L13" t="s">
         <v>28</v>
       </c>
-      <c r="AA13" s="1" t="s">
+      <c r="AB13" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>140</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1585,7 +1600,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{377959F3-1E32-48D5-BD0D-DAFF6699BAE0}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB1048576" xr:uid="{99999286-3ED4-4B5C-B2BF-6EDC933F7B52}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC1048576" xr:uid="{99999286-3ED4-4B5C-B2BF-6EDC933F7B52}">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{89425058-0C05-4809-93A2-EBBE8CA5B4F6}">
@@ -1598,34 +1613,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
-  <dimension ref="A1:AJ11"/>
+  <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA4" sqref="AA4"/>
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="90.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="44.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" style="1"/>
-    <col min="29" max="29" width="71.85546875" customWidth="1"/>
-    <col min="30" max="30" width="63.85546875" customWidth="1"/>
-    <col min="31" max="31" width="59.42578125" customWidth="1"/>
-    <col min="32" max="32" width="60.140625" customWidth="1"/>
-    <col min="33" max="33" width="61.42578125" customWidth="1"/>
-    <col min="34" max="34" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" customWidth="1"/>
+    <col min="3" max="3" width="90.109375" customWidth="1"/>
+    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.88671875" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="28" max="28" width="9.109375" style="1"/>
+    <col min="30" max="30" width="71.88671875" customWidth="1"/>
+    <col min="31" max="31" width="63.88671875" customWidth="1"/>
+    <col min="32" max="32" width="59.44140625" customWidth="1"/>
+    <col min="33" max="33" width="60.109375" customWidth="1"/>
+    <col min="34" max="34" width="61.44140625" customWidth="1"/>
+    <col min="35" max="35" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1705,37 +1720,40 @@
         <v>135</v>
       </c>
       <c r="AA1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AB1" t="s">
         <v>136</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>138</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>105</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>107</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>106</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>108</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>109</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>110</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>137</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1009</v>
       </c>
@@ -1760,23 +1778,23 @@
       <c r="L2" t="s">
         <v>29</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>140</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>38</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>39</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1006</v>
       </c>
@@ -1807,17 +1825,20 @@
       <c r="L3" t="s">
         <v>28</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AA3">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>140</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -1842,17 +1863,17 @@
       <c r="L4" t="s">
         <v>31</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>140</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>42</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1001</v>
       </c>
@@ -1880,17 +1901,17 @@
       <c r="L5" t="s">
         <v>31</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>140</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>205</v>
       </c>
@@ -1912,14 +1933,17 @@
       <c r="L6" t="s">
         <v>29</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AA6">
+        <v>3</v>
+      </c>
+      <c r="AC6" t="s">
         <v>140</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>205</v>
       </c>
@@ -1941,17 +1965,20 @@
       <c r="L7" t="s">
         <v>29</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AA7">
+        <v>2</v>
+      </c>
+      <c r="AB7" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>140</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>205</v>
       </c>
@@ -1973,17 +2000,17 @@
       <c r="L8" t="s">
         <v>29</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>140</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>205</v>
       </c>
@@ -2005,17 +2032,17 @@
       <c r="L9" t="s">
         <v>29</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>140</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>205</v>
       </c>
@@ -2037,17 +2064,17 @@
       <c r="L10" t="s">
         <v>29</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AB10" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>140</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>123</v>
       </c>
@@ -2066,13 +2093,13 @@
       <c r="L11" t="s">
         <v>29</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>141</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>152</v>
       </c>
     </row>
@@ -2085,13 +2112,13 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:J11 F13:J1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
       <formula1>Subcategories</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Z11 L13:Z1048576" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:Z1048576 L2:Z11" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
       <formula1>Tags</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K11 K13:K1048576" xr:uid="{D0466454-C892-488E-AA3C-A206F5B6F670}">
       <formula1>DesignType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AB2:AB11 AB13:AB1048576" xr:uid="{9EF19CFE-4BEB-4B6E-9893-F1BFEBCAA2B4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC11 AC13:AC1048576" xr:uid="{9EF19CFE-4BEB-4B6E-9893-F1BFEBCAA2B4}">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{510EF69A-8273-4570-9E7F-349E731D2D60}">
@@ -2111,132 +2138,132 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>184</v>
       </c>
@@ -2254,12 +2281,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2267,7 +2294,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2275,7 +2302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2283,7 +2310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2291,7 +2318,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -2299,7 +2326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2307,7 +2334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2315,7 +2342,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -2342,14 +2369,14 @@
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" customWidth="1"/>
-    <col min="3" max="3" width="55.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="55.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2360,7 +2387,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -2372,7 +2399,7 @@
         <v>Quick Search &gt; New Designs</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -2384,7 +2411,7 @@
         <v>Quick Search &gt; Best Sellers</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2396,7 +2423,7 @@
         <v>Quick Search &gt; Staff Favorites</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -2408,7 +2435,7 @@
         <v>Quick Search &gt; Classics</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2420,7 +2447,7 @@
         <v>Quick Search &gt; Patriotic</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2432,7 +2459,7 @@
         <v>Quick Search &gt; Economy</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2444,7 +2471,7 @@
         <v>Quick Search &gt; Ladies</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2456,7 +2483,7 @@
         <v>Event/Awareness &gt; Strike &amp; Negotiations</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -2468,7 +2495,7 @@
         <v>Event/Awareness &gt; Golf</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -2480,7 +2507,7 @@
         <v>Event/Awareness &gt; Picnics</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2492,7 +2519,7 @@
         <v>Event/Awareness &gt; Anniversary</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2504,7 +2531,7 @@
         <v>Event/Awareness &gt; Political</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -2516,7 +2543,7 @@
         <v>Event/Awareness &gt; Breast Cancer</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2528,7 +2555,7 @@
         <v>Holiday &gt; Labor Day</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -2540,7 +2567,7 @@
         <v>Holiday &gt; St. Patrick's Day</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -2552,7 +2579,7 @@
         <v>Holiday &gt; Veterans Day</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -2564,7 +2591,7 @@
         <v>Union Specific &gt; International Logos</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -2576,7 +2603,7 @@
         <v>Union Specific &gt; APWU</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -2588,7 +2615,7 @@
         <v>Union Specific &gt; BAC</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2600,7 +2627,7 @@
         <v>Union Specific &gt; Boilermakers</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -2612,7 +2639,7 @@
         <v>Union Specific &gt; Carpenters</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -2624,7 +2651,7 @@
         <v>Union Specific &gt; CWA</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -2636,7 +2663,7 @@
         <v>Union Specific &gt; Electrical Workers</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -2648,7 +2675,7 @@
         <v>Union Specific &gt; IAFF</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2660,7 +2687,7 @@
         <v>Union Specific &gt; IAM</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -2672,7 +2699,7 @@
         <v>Union Specific &gt; IATSE</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2684,7 +2711,7 @@
         <v>Union Specific &gt; Ironworkers</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -2696,7 +2723,7 @@
         <v>Union Specific &gt; Heat &amp; Frost Insulators</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2708,7 +2735,7 @@
         <v>Union Specific &gt; IUEC</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -2720,7 +2747,7 @@
         <v>Union Specific &gt; IUOE</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -2732,7 +2759,7 @@
         <v>Union Specific &gt; IUPAT</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -2744,7 +2771,7 @@
         <v>Union Specific &gt; Laborers</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2756,7 +2783,7 @@
         <v>Union Specific &gt; Mailhandlers</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -2768,7 +2795,7 @@
         <v>Union Specific &gt; NATCA</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -2780,7 +2807,7 @@
         <v>Union Specific &gt; NALC</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2792,7 +2819,7 @@
         <v>Union Specific &gt; NEA</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -2804,7 +2831,7 @@
         <v>Union Specific &gt; OPCMIA</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -2816,7 +2843,7 @@
         <v>Union Specific &gt; OPEIU</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2828,7 +2855,7 @@
         <v>Union Specific &gt; PASS</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -2840,7 +2867,7 @@
         <v>Union Specific &gt; Nurses</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -2852,7 +2879,7 @@
         <v>Union Specific &gt; Roofers</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -2864,7 +2891,7 @@
         <v>Union Specific &gt; SEIU</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2876,7 +2903,7 @@
         <v>Union Specific &gt; SMART</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -2888,7 +2915,7 @@
         <v>Union Specific &gt; Teamsters</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -2900,7 +2927,7 @@
         <v>Union Specific &gt; UA</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2912,7 +2939,7 @@
         <v>Union Specific &gt; UAW</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2924,7 +2951,7 @@
         <v>Union Specific &gt; UWUA</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -2936,7 +2963,7 @@
         <v>Union Specific &gt; USW</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -2948,7 +2975,7 @@
         <v>Location Specific &gt; Sleeve</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2960,7 +2987,7 @@
         <v>Location Specific &gt; Oversize</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -2972,7 +2999,7 @@
         <v>Location Specific &gt; Youth/Kids</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -2984,7 +3011,7 @@
         <v>International Union Logos &gt; APWU</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -2996,7 +3023,7 @@
         <v>International Union Logos &gt; BAC</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -3008,7 +3035,7 @@
         <v>International Union Logos &gt; Boilermakers</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -3020,7 +3047,7 @@
         <v>International Union Logos &gt; Carpenters</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -3032,7 +3059,7 @@
         <v>International Union Logos &gt; CWA</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -3044,7 +3071,7 @@
         <v>International Union Logos &gt; Electrical Workers</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -3056,7 +3083,7 @@
         <v>International Union Logos &gt; IAFF</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -3068,7 +3095,7 @@
         <v>International Union Logos &gt; IAM</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3080,7 +3107,7 @@
         <v>International Union Logos &gt; IATSE</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -3092,7 +3119,7 @@
         <v>International Union Logos &gt; Ironworkers</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -3104,7 +3131,7 @@
         <v>International Union Logos &gt; Heat &amp; Frost Insulators</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -3116,7 +3143,7 @@
         <v>International Union Logos &gt; IUEC</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -3128,7 +3155,7 @@
         <v>International Union Logos &gt; IUOE</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -3140,7 +3167,7 @@
         <v>International Union Logos &gt; IUPAT</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -3152,7 +3179,7 @@
         <v>International Union Logos &gt; Laborers</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -3164,7 +3191,7 @@
         <v>International Union Logos &gt; Mailhandlers</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -3176,7 +3203,7 @@
         <v>International Union Logos &gt; NATCA</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -3188,7 +3215,7 @@
         <v>International Union Logos &gt; NALC</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -3200,7 +3227,7 @@
         <v>International Union Logos &gt; NEA</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -3212,7 +3239,7 @@
         <v>International Union Logos &gt; OPCMIA</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -3224,7 +3251,7 @@
         <v>International Union Logos &gt; OPEIU</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -3236,7 +3263,7 @@
         <v>International Union Logos &gt; PASS</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -3248,7 +3275,7 @@
         <v>International Union Logos &gt; Nurses</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -3260,7 +3287,7 @@
         <v>International Union Logos &gt; Roofers</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3272,7 +3299,7 @@
         <v>International Union Logos &gt; SEIU</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -3284,7 +3311,7 @@
         <v>International Union Logos &gt; SMART</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>89</v>
       </c>
@@ -3296,7 +3323,7 @@
         <v>International Union Logos &gt; Teamsters</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -3308,7 +3335,7 @@
         <v>International Union Logos &gt; UA</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -3320,7 +3347,7 @@
         <v>International Union Logos &gt; UAW</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>92</v>
       </c>
@@ -3332,7 +3359,7 @@
         <v>International Union Logos &gt; UWUA</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>93</v>
       </c>
@@ -3344,7 +3371,7 @@
         <v>International Union Logos &gt; USW</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>122</v>
       </c>
@@ -3356,7 +3383,7 @@
         <v>Inspiration Board &gt; Hats/Beanies</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>123</v>
       </c>
@@ -3368,7 +3395,7 @@
         <v>Inspiration Board &gt; Chest/Sleeve</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>124</v>
       </c>
@@ -3380,7 +3407,7 @@
         <v>Inspiration Board &gt; Full Size Embroidery</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>125</v>
       </c>
@@ -3410,19 +3437,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>111</v>
       </c>
@@ -3440,19 +3467,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>111</v>
       </c>
@@ -3470,34 +3497,34 @@
       <selection activeCell="A2" sqref="A2:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3515,19 +3542,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Improve quote request email
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E0348B-E86F-456C-AED8-026109A6775B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177333F6-C0EB-4518-AB18-87F0B5499827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="192">
   <si>
     <t>Name</t>
   </si>
@@ -499,18 +499,6 @@
     <t>Union Specific &gt; USW</t>
   </si>
   <si>
-    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205.jpg</t>
-  </si>
-  <si>
-    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (2).jpg</t>
-  </si>
-  <si>
-    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (3).jpg</t>
-  </si>
-  <si>
-    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (4).jpg</t>
-  </si>
-  <si>
     <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (5).jpg</t>
   </si>
   <si>
@@ -623,6 +611,24 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Existing Designs/Downloaded Images 12-13-2023/205.jpg</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Existing Designs/Downloaded Images 12-13-2023/205 (2).jpg</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Existing Designs/Downloaded Images 12-13-2023/205 (3).jpg</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Existing Designs/Downloaded Images 12-13-2023/205 (4).jpg</t>
+  </si>
+  <si>
+    <t>/Marketing/Website/Design Library/Existing Designs/Downloaded Images 12-13-2023/205 (5).jpg</t>
+  </si>
+  <si>
+    <t>Holiday &gt; St. Patrick's Day</t>
   </si>
 </sst>
 </file>
@@ -992,8 +998,8 @@
   <dimension ref="A1:AK13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="U1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA12" sqref="AA12"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1033,10 +1039,10 @@
         <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1096,7 +1102,7 @@
         <v>135</v>
       </c>
       <c r="AA1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="AB1" t="s">
         <v>136</v>
@@ -1140,7 +1146,7 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -1161,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AC2" t="s">
         <v>140</v>
@@ -1184,13 +1190,13 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K3" t="s">
         <v>12</v>
@@ -1205,7 +1211,7 @@
         <v>30</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC3" t="s">
         <v>140</v>
@@ -1225,13 +1231,13 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K4" t="s">
         <v>12</v>
@@ -1240,13 +1246,13 @@
         <v>28</v>
       </c>
       <c r="AB4" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC4" t="s">
         <v>140</v>
       </c>
       <c r="AD4" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="AE4" t="s">
         <v>39</v>
@@ -1275,7 +1281,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -1296,7 +1302,7 @@
         <v>27</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC5" t="s">
         <v>140</v>
@@ -1316,13 +1322,13 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K6" t="s">
         <v>12</v>
@@ -1334,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AC6" t="s">
         <v>140</v>
@@ -1354,13 +1360,13 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K7" t="s">
         <v>12</v>
@@ -1369,7 +1375,7 @@
         <v>27</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC7" t="s">
         <v>140</v>
@@ -1389,13 +1395,13 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K8" t="s">
         <v>12</v>
@@ -1404,7 +1410,7 @@
         <v>27</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AC8" t="s">
         <v>140</v>
@@ -1424,13 +1430,13 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K9" t="s">
         <v>12</v>
@@ -1439,7 +1445,7 @@
         <v>30</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC9" t="s">
         <v>140</v>
@@ -1459,13 +1465,13 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K10" t="s">
         <v>12</v>
@@ -1477,7 +1483,7 @@
         <v>2</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC10" t="s">
         <v>140</v>
@@ -1497,13 +1503,13 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K11" t="s">
         <v>12</v>
@@ -1512,7 +1518,7 @@
         <v>31</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC11" t="s">
         <v>140</v>
@@ -1532,13 +1538,13 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="F12" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="K12" t="s">
         <v>12</v>
@@ -1547,7 +1553,7 @@
         <v>27</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AC12" t="s">
         <v>140</v>
@@ -1561,28 +1567,31 @@
         <v>549</v>
       </c>
       <c r="B13" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13" t="s">
-        <v>157</v>
+        <v>153</v>
+      </c>
+      <c r="G13" t="s">
+        <v>191</v>
       </c>
       <c r="L13" t="s">
         <v>28</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC13" t="s">
         <v>140</v>
       </c>
       <c r="AD13" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1616,8 +1625,8 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA9" sqref="AA9"/>
+      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1657,10 +1666,10 @@
         <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1720,7 +1729,7 @@
         <v>135</v>
       </c>
       <c r="AA1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="AB1" t="s">
         <v>136</v>
@@ -1764,7 +1773,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -1779,7 +1788,7 @@
         <v>29</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC2" t="s">
         <v>140</v>
@@ -1805,7 +1814,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -1829,7 +1838,7 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC3" t="s">
         <v>140</v>
@@ -1849,7 +1858,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1884,7 +1893,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -1902,7 +1911,7 @@
         <v>31</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC5" t="s">
         <v>140</v>
@@ -1919,7 +1928,7 @@
         <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -1940,7 +1949,7 @@
         <v>140</v>
       </c>
       <c r="AD6" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.3">
@@ -1951,7 +1960,7 @@
         <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -1969,13 +1978,13 @@
         <v>2</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC7" t="s">
         <v>140</v>
       </c>
       <c r="AD7" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.3">
@@ -1986,7 +1995,7 @@
         <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -2001,13 +2010,13 @@
         <v>29</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC8" t="s">
         <v>140</v>
       </c>
       <c r="AD8" t="s">
-        <v>150</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.3">
@@ -2018,7 +2027,7 @@
         <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -2033,13 +2042,13 @@
         <v>29</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC9" t="s">
         <v>140</v>
       </c>
       <c r="AD9" t="s">
-        <v>151</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.3">
@@ -2050,7 +2059,7 @@
         <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -2065,13 +2074,13 @@
         <v>29</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC10" t="s">
         <v>140</v>
       </c>
       <c r="AD10" t="s">
-        <v>152</v>
+        <v>190</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.3">
@@ -2079,28 +2088,28 @@
         <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="L11" t="s">
         <v>29</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="AC11" t="s">
         <v>141</v>
       </c>
       <c r="AD11" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2145,127 +2154,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add exclude prioritized param
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177333F6-C0EB-4518-AB18-87F0B5499827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A12286-C8CC-42EF-BA3C-55CC0CDBF7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="192">
   <si>
     <t>Name</t>
   </si>
@@ -995,34 +995,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
-  <dimension ref="A1:AK13"/>
+  <dimension ref="A1:AL13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G13" sqref="G13"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="90.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" customWidth="1"/>
-    <col min="6" max="6" width="27.44140625" customWidth="1"/>
-    <col min="7" max="7" width="29.5546875" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="28" max="28" width="9.109375" style="1"/>
-    <col min="30" max="30" width="71.88671875" customWidth="1"/>
-    <col min="31" max="31" width="63.88671875" customWidth="1"/>
-    <col min="32" max="32" width="59.44140625" customWidth="1"/>
-    <col min="33" max="33" width="60.109375" customWidth="1"/>
-    <col min="34" max="34" width="61.44140625" customWidth="1"/>
-    <col min="35" max="35" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="90.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="23.85546875" customWidth="1"/>
+    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" style="1"/>
+    <col min="31" max="31" width="71.85546875" customWidth="1"/>
+    <col min="32" max="32" width="63.85546875" customWidth="1"/>
+    <col min="33" max="33" width="59.42578125" customWidth="1"/>
+    <col min="34" max="34" width="60.140625" customWidth="1"/>
+    <col min="35" max="35" width="61.42578125" customWidth="1"/>
+    <col min="36" max="36" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1039,103 +1039,106 @@
         <v>49</v>
       </c>
       <c r="F1" t="s">
+        <v>185</v>
+      </c>
+      <c r="G1" t="s">
         <v>154</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>155</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>32</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>126</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>127</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>128</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>129</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>130</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>131</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>132</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>133</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>134</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>135</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>185</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>136</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>138</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>105</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>107</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>106</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>108</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>109</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>110</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>137</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1025</v>
       </c>
@@ -1151,35 +1154,35 @@
       <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>97</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>112</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>12</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>30</v>
       </c>
-      <c r="AA2">
+      <c r="AB2">
         <v>3</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>140</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>37</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1003</v>
       </c>
@@ -1195,32 +1198,32 @@
       <c r="E3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>183</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>12</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>27</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>28</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>30</v>
       </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>140</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1236,41 +1239,41 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>183</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>12</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>28</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>140</v>
       </c>
-      <c r="AD4" t="s">
+      <c r="AE4" t="s">
         <v>184</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>39</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>38</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>42</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>41</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1286,32 +1289,32 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>99</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>101</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>12</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>27</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>140</v>
       </c>
-      <c r="AD5" t="s">
+      <c r="AE5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1012</v>
       </c>
@@ -1327,29 +1330,29 @@
       <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>183</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>12</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>28</v>
       </c>
-      <c r="AA6">
+      <c r="AB6">
         <v>1</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>140</v>
       </c>
-      <c r="AD6" t="s">
+      <c r="AE6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1013</v>
       </c>
@@ -1365,26 +1368,26 @@
       <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>183</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>12</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>27</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>140</v>
       </c>
-      <c r="AD7" t="s">
+      <c r="AE7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1014</v>
       </c>
@@ -1400,26 +1403,26 @@
       <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>183</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>12</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>27</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AC8" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>140</v>
       </c>
-      <c r="AD8" t="s">
+      <c r="AE8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1015</v>
       </c>
@@ -1435,26 +1438,26 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>183</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>12</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>30</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>140</v>
       </c>
-      <c r="AD9" t="s">
+      <c r="AE9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1016</v>
       </c>
@@ -1470,29 +1473,29 @@
       <c r="E10" t="s">
         <v>14</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>183</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>12</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>29</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <v>2</v>
       </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AC10" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>140</v>
       </c>
-      <c r="AD10" t="s">
+      <c r="AE10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1017</v>
       </c>
@@ -1508,26 +1511,26 @@
       <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>183</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>12</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>31</v>
       </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AC11" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>140</v>
       </c>
-      <c r="AD11" t="s">
+      <c r="AE11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1018</v>
       </c>
@@ -1543,26 +1546,26 @@
       <c r="E12" t="s">
         <v>14</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>183</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>12</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>27</v>
       </c>
-      <c r="AB12" s="1" t="s">
+      <c r="AC12" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>140</v>
       </c>
-      <c r="AD12" t="s">
+      <c r="AE12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>549</v>
       </c>
@@ -1575,41 +1578,44 @@
       <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
         <v>153</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>191</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>28</v>
       </c>
-      <c r="AB13" s="1" t="s">
+      <c r="AC13" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>140</v>
       </c>
-      <c r="AD13" t="s">
+      <c r="AE13" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K1048576" xr:uid="{A61431EB-F298-41CC-8A14-D29D28DE34A1}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576" xr:uid="{A61431EB-F298-41CC-8A14-D29D28DE34A1}">
       <formula1>DesignType</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:Z1048576" xr:uid="{0F9108B0-AF43-4436-8202-F35401506D80}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:AA1048576" xr:uid="{0F9108B0-AF43-4436-8202-F35401506D80}">
       <formula1>Tags</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:J1048576" xr:uid="{358D683C-DBF6-4E6F-8311-F37F9C488CA5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:K1048576" xr:uid="{358D683C-DBF6-4E6F-8311-F37F9C488CA5}">
       <formula1>Subcategories</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{377959F3-1E32-48D5-BD0D-DAFF6699BAE0}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2:AC1048576" xr:uid="{99999286-3ED4-4B5C-B2BF-6EDC933F7B52}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD1048576" xr:uid="{99999286-3ED4-4B5C-B2BF-6EDC933F7B52}">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{89425058-0C05-4809-93A2-EBBE8CA5B4F6}">
@@ -1629,27 +1635,27 @@
       <selection pane="topRight" activeCell="AD14" sqref="AD14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" customWidth="1"/>
-    <col min="3" max="3" width="90.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" customWidth="1"/>
-    <col min="6" max="6" width="44.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="28" max="28" width="9.109375" style="1"/>
-    <col min="30" max="30" width="71.88671875" customWidth="1"/>
-    <col min="31" max="31" width="63.88671875" customWidth="1"/>
-    <col min="32" max="32" width="59.44140625" customWidth="1"/>
-    <col min="33" max="33" width="60.109375" customWidth="1"/>
-    <col min="34" max="34" width="61.44140625" customWidth="1"/>
-    <col min="35" max="35" width="23.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="90.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="1"/>
+    <col min="30" max="30" width="71.85546875" customWidth="1"/>
+    <col min="31" max="31" width="63.85546875" customWidth="1"/>
+    <col min="32" max="32" width="59.42578125" customWidth="1"/>
+    <col min="33" max="33" width="60.140625" customWidth="1"/>
+    <col min="34" max="34" width="61.42578125" customWidth="1"/>
+    <col min="35" max="35" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1762,7 +1768,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1009</v>
       </c>
@@ -1803,7 +1809,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1006</v>
       </c>
@@ -1847,7 +1853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1000</v>
       </c>
@@ -1882,7 +1888,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1001</v>
       </c>
@@ -1920,7 +1926,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>205</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>205</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>205</v>
       </c>
@@ -2019,7 +2025,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>205</v>
       </c>
@@ -2051,7 +2057,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>205</v>
       </c>
@@ -2083,7 +2089,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>123</v>
       </c>
@@ -2147,132 +2153,132 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="23" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="25" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>180</v>
       </c>
@@ -2290,12 +2296,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.88671875" customWidth="1"/>
+    <col min="1" max="1" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2303,7 +2309,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -2311,7 +2317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -2319,7 +2325,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2327,7 +2333,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -2335,7 +2341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2343,7 +2349,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2351,7 +2357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -2378,14 +2384,14 @@
       <selection activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="55.109375" customWidth="1"/>
+    <col min="1" max="1" width="37.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="55.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2396,7 +2402,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -2408,7 +2414,7 @@
         <v>Quick Search &gt; New Designs</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>Quick Search &gt; Best Sellers</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -2432,7 +2438,7 @@
         <v>Quick Search &gt; Staff Favorites</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -2444,7 +2450,7 @@
         <v>Quick Search &gt; Classics</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -2456,7 +2462,7 @@
         <v>Quick Search &gt; Patriotic</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -2468,7 +2474,7 @@
         <v>Quick Search &gt; Economy</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -2480,7 +2486,7 @@
         <v>Quick Search &gt; Ladies</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2492,7 +2498,7 @@
         <v>Event/Awareness &gt; Strike &amp; Negotiations</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -2504,7 +2510,7 @@
         <v>Event/Awareness &gt; Golf</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -2516,7 +2522,7 @@
         <v>Event/Awareness &gt; Picnics</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2528,7 +2534,7 @@
         <v>Event/Awareness &gt; Anniversary</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -2540,7 +2546,7 @@
         <v>Event/Awareness &gt; Political</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -2552,7 +2558,7 @@
         <v>Event/Awareness &gt; Breast Cancer</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -2564,7 +2570,7 @@
         <v>Holiday &gt; Labor Day</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>62</v>
       </c>
@@ -2576,7 +2582,7 @@
         <v>Holiday &gt; St. Patrick's Day</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -2588,7 +2594,7 @@
         <v>Holiday &gt; Veterans Day</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>64</v>
       </c>
@@ -2600,7 +2606,7 @@
         <v>Union Specific &gt; International Logos</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>65</v>
       </c>
@@ -2612,7 +2618,7 @@
         <v>Union Specific &gt; APWU</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -2624,7 +2630,7 @@
         <v>Union Specific &gt; BAC</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -2636,7 +2642,7 @@
         <v>Union Specific &gt; Boilermakers</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>68</v>
       </c>
@@ -2648,7 +2654,7 @@
         <v>Union Specific &gt; Carpenters</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -2660,7 +2666,7 @@
         <v>Union Specific &gt; CWA</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>70</v>
       </c>
@@ -2672,7 +2678,7 @@
         <v>Union Specific &gt; Electrical Workers</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>71</v>
       </c>
@@ -2684,7 +2690,7 @@
         <v>Union Specific &gt; IAFF</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>72</v>
       </c>
@@ -2696,7 +2702,7 @@
         <v>Union Specific &gt; IAM</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>73</v>
       </c>
@@ -2708,7 +2714,7 @@
         <v>Union Specific &gt; IATSE</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2720,7 +2726,7 @@
         <v>Union Specific &gt; Ironworkers</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>75</v>
       </c>
@@ -2732,7 +2738,7 @@
         <v>Union Specific &gt; Heat &amp; Frost Insulators</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>76</v>
       </c>
@@ -2744,7 +2750,7 @@
         <v>Union Specific &gt; IUEC</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -2756,7 +2762,7 @@
         <v>Union Specific &gt; IUOE</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -2768,7 +2774,7 @@
         <v>Union Specific &gt; IUPAT</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>78</v>
       </c>
@@ -2780,7 +2786,7 @@
         <v>Union Specific &gt; Laborers</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2792,7 +2798,7 @@
         <v>Union Specific &gt; Mailhandlers</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -2804,7 +2810,7 @@
         <v>Union Specific &gt; NATCA</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>81</v>
       </c>
@@ -2816,7 +2822,7 @@
         <v>Union Specific &gt; NALC</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>82</v>
       </c>
@@ -2828,7 +2834,7 @@
         <v>Union Specific &gt; NEA</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>83</v>
       </c>
@@ -2840,7 +2846,7 @@
         <v>Union Specific &gt; OPCMIA</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -2852,7 +2858,7 @@
         <v>Union Specific &gt; OPEIU</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>85</v>
       </c>
@@ -2864,7 +2870,7 @@
         <v>Union Specific &gt; PASS</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -2876,7 +2882,7 @@
         <v>Union Specific &gt; Nurses</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>87</v>
       </c>
@@ -2888,7 +2894,7 @@
         <v>Union Specific &gt; Roofers</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>16</v>
       </c>
@@ -2900,7 +2906,7 @@
         <v>Union Specific &gt; SEIU</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>88</v>
       </c>
@@ -2912,7 +2918,7 @@
         <v>Union Specific &gt; SMART</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>89</v>
       </c>
@@ -2924,7 +2930,7 @@
         <v>Union Specific &gt; Teamsters</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>90</v>
       </c>
@@ -2936,7 +2942,7 @@
         <v>Union Specific &gt; UA</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>91</v>
       </c>
@@ -2948,7 +2954,7 @@
         <v>Union Specific &gt; UAW</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>92</v>
       </c>
@@ -2960,7 +2966,7 @@
         <v>Union Specific &gt; UWUA</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>93</v>
       </c>
@@ -2972,7 +2978,7 @@
         <v>Union Specific &gt; USW</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>94</v>
       </c>
@@ -2984,7 +2990,7 @@
         <v>Location Specific &gt; Sleeve</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>95</v>
       </c>
@@ -2996,7 +3002,7 @@
         <v>Location Specific &gt; Oversize</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>96</v>
       </c>
@@ -3008,7 +3014,7 @@
         <v>Location Specific &gt; Youth/Kids</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>65</v>
       </c>
@@ -3020,7 +3026,7 @@
         <v>International Union Logos &gt; APWU</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>66</v>
       </c>
@@ -3032,7 +3038,7 @@
         <v>International Union Logos &gt; BAC</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>67</v>
       </c>
@@ -3044,7 +3050,7 @@
         <v>International Union Logos &gt; Boilermakers</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -3056,7 +3062,7 @@
         <v>International Union Logos &gt; Carpenters</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>69</v>
       </c>
@@ -3068,7 +3074,7 @@
         <v>International Union Logos &gt; CWA</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -3080,7 +3086,7 @@
         <v>International Union Logos &gt; Electrical Workers</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>71</v>
       </c>
@@ -3092,7 +3098,7 @@
         <v>International Union Logos &gt; IAFF</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>72</v>
       </c>
@@ -3104,7 +3110,7 @@
         <v>International Union Logos &gt; IAM</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>73</v>
       </c>
@@ -3116,7 +3122,7 @@
         <v>International Union Logos &gt; IATSE</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -3128,7 +3134,7 @@
         <v>International Union Logos &gt; Ironworkers</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>75</v>
       </c>
@@ -3140,7 +3146,7 @@
         <v>International Union Logos &gt; Heat &amp; Frost Insulators</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>76</v>
       </c>
@@ -3152,7 +3158,7 @@
         <v>International Union Logos &gt; IUEC</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>77</v>
       </c>
@@ -3164,7 +3170,7 @@
         <v>International Union Logos &gt; IUOE</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>17</v>
       </c>
@@ -3176,7 +3182,7 @@
         <v>International Union Logos &gt; IUPAT</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>78</v>
       </c>
@@ -3188,7 +3194,7 @@
         <v>International Union Logos &gt; Laborers</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>79</v>
       </c>
@@ -3200,7 +3206,7 @@
         <v>International Union Logos &gt; Mailhandlers</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>80</v>
       </c>
@@ -3212,7 +3218,7 @@
         <v>International Union Logos &gt; NATCA</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -3224,7 +3230,7 @@
         <v>International Union Logos &gt; NALC</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>82</v>
       </c>
@@ -3236,7 +3242,7 @@
         <v>International Union Logos &gt; NEA</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>83</v>
       </c>
@@ -3248,7 +3254,7 @@
         <v>International Union Logos &gt; OPCMIA</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>84</v>
       </c>
@@ -3260,7 +3266,7 @@
         <v>International Union Logos &gt; OPEIU</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>85</v>
       </c>
@@ -3272,7 +3278,7 @@
         <v>International Union Logos &gt; PASS</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>86</v>
       </c>
@@ -3284,7 +3290,7 @@
         <v>International Union Logos &gt; Nurses</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>87</v>
       </c>
@@ -3296,7 +3302,7 @@
         <v>International Union Logos &gt; Roofers</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>16</v>
       </c>
@@ -3308,7 +3314,7 @@
         <v>International Union Logos &gt; SEIU</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -3320,7 +3326,7 @@
         <v>International Union Logos &gt; SMART</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>89</v>
       </c>
@@ -3332,7 +3338,7 @@
         <v>International Union Logos &gt; Teamsters</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -3344,7 +3350,7 @@
         <v>International Union Logos &gt; UA</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -3356,7 +3362,7 @@
         <v>International Union Logos &gt; UAW</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>92</v>
       </c>
@@ -3368,7 +3374,7 @@
         <v>International Union Logos &gt; UWUA</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>93</v>
       </c>
@@ -3380,7 +3386,7 @@
         <v>International Union Logos &gt; USW</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>122</v>
       </c>
@@ -3392,7 +3398,7 @@
         <v>Inspiration Board &gt; Hats/Beanies</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>123</v>
       </c>
@@ -3404,7 +3410,7 @@
         <v>Inspiration Board &gt; Chest/Sleeve</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>124</v>
       </c>
@@ -3416,7 +3422,7 @@
         <v>Inspiration Board &gt; Full Size Embroidery</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>125</v>
       </c>
@@ -3446,19 +3452,19 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>111</v>
       </c>
@@ -3476,19 +3482,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>111</v>
       </c>
@@ -3506,34 +3512,34 @@
       <selection activeCell="A2" sqref="A2:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -3551,19 +3557,19 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>111</v>
       </c>

</xml_diff>

<commit_message>
Change to new url
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A12286-C8CC-42EF-BA3C-55CC0CDBF7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EA3147-D0B7-40DD-88AE-6964CF66F429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="191">
   <si>
     <t>Name</t>
   </si>
@@ -626,9 +626,6 @@
   </si>
   <si>
     <t>/Marketing/Website/Design Library/Existing Designs/Downloaded Images 12-13-2023/205 (5).jpg</t>
-  </si>
-  <si>
-    <t>Holiday &gt; St. Patrick's Day</t>
   </si>
 </sst>
 </file>
@@ -998,8 +995,8 @@
   <dimension ref="A1:AL13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E27" sqref="E27"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,9 +1580,6 @@
       </c>
       <c r="G13" t="s">
         <v>153</v>
-      </c>
-      <c r="H13" t="s">
-        <v>191</v>
       </c>
       <c r="M13" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Add image url to design schema
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30EA3147-D0B7-40DD-88AE-6964CF66F429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E6FE70-D2C4-4D39-B241-5BF43D39E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -626,13 +626,19 @@
   </si>
   <si>
     <t>/Marketing/Website/Design Library/Existing Designs/Downloaded Images 12-13-2023/205 (5).jpg</t>
+  </si>
+  <si>
+    <t>Image URL</t>
+  </si>
+  <si>
+    <t>https://www.imagepointe.com/wp-content/uploads/2024/02/1732-darks.png</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -649,6 +655,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -671,15 +685,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -992,11 +1009,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
-  <dimension ref="A1:AL13"/>
+  <dimension ref="A1:AM13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H16" sqref="H16"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AE7" sqref="AE7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,15 +1028,16 @@
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" customWidth="1"/>
     <col min="29" max="29" width="9.140625" style="1"/>
-    <col min="31" max="31" width="71.85546875" customWidth="1"/>
-    <col min="32" max="32" width="63.85546875" customWidth="1"/>
-    <col min="33" max="33" width="59.42578125" customWidth="1"/>
-    <col min="34" max="34" width="60.140625" customWidth="1"/>
-    <col min="35" max="35" width="61.42578125" customWidth="1"/>
-    <col min="36" max="36" width="23.140625" customWidth="1"/>
+    <col min="31" max="31" width="71.140625" customWidth="1"/>
+    <col min="32" max="32" width="71.85546875" customWidth="1"/>
+    <col min="33" max="33" width="63.85546875" customWidth="1"/>
+    <col min="34" max="34" width="59.42578125" customWidth="1"/>
+    <col min="35" max="35" width="60.140625" customWidth="1"/>
+    <col min="36" max="36" width="61.42578125" customWidth="1"/>
+    <col min="37" max="37" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -1111,31 +1129,34 @@
         <v>138</v>
       </c>
       <c r="AE1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AF1" t="s">
         <v>105</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>107</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>106</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>108</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>109</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>110</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>137</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1025</v>
       </c>
@@ -1172,14 +1193,17 @@
       <c r="AD2" t="s">
         <v>140</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AE2" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="AF2" t="s">
         <v>37</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1003</v>
       </c>
@@ -1216,11 +1240,11 @@
       <c r="AD3" t="s">
         <v>140</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1251,26 +1275,26 @@
       <c r="AD4" t="s">
         <v>140</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>184</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AG4" t="s">
         <v>39</v>
       </c>
-      <c r="AG4" t="s">
+      <c r="AH4" t="s">
         <v>38</v>
       </c>
-      <c r="AH4" t="s">
+      <c r="AI4" t="s">
         <v>42</v>
       </c>
-      <c r="AI4" t="s">
+      <c r="AJ4" t="s">
         <v>41</v>
       </c>
-      <c r="AJ4" t="s">
+      <c r="AK4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -1307,11 +1331,11 @@
       <c r="AD5" t="s">
         <v>140</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1012</v>
       </c>
@@ -1345,11 +1369,11 @@
       <c r="AD6" t="s">
         <v>140</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1013</v>
       </c>
@@ -1380,11 +1404,11 @@
       <c r="AD7" t="s">
         <v>140</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1014</v>
       </c>
@@ -1415,11 +1439,11 @@
       <c r="AD8" t="s">
         <v>140</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1015</v>
       </c>
@@ -1450,11 +1474,11 @@
       <c r="AD9" t="s">
         <v>140</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1016</v>
       </c>
@@ -1488,11 +1512,11 @@
       <c r="AD10" t="s">
         <v>140</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1017</v>
       </c>
@@ -1523,11 +1547,11 @@
       <c r="AD11" t="s">
         <v>140</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1018</v>
       </c>
@@ -1558,11 +1582,11 @@
       <c r="AD12" t="s">
         <v>140</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>549</v>
       </c>
@@ -1590,7 +1614,7 @@
       <c r="AD13" t="s">
         <v>140</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>152</v>
       </c>
     </row>
@@ -1609,13 +1633,16 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576" xr:uid="{377959F3-1E32-48D5-BD0D-DAFF6699BAE0}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD1048576" xr:uid="{99999286-3ED4-4B5C-B2BF-6EDC933F7B52}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2:AD1048576 AE3:AE1048576" xr:uid="{99999286-3ED4-4B5C-B2BF-6EDC933F7B52}">
       <formula1>Status</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{89425058-0C05-4809-93A2-EBBE8CA5B4F6}">
       <formula1>Colors</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="AE2" r:id="rId1" xr:uid="{98281F5D-64D5-4743-B979-4457E043A43C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix second fetch attempt after access token update; fix category filtering logic
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E6FE70-D2C4-4D39-B241-5BF43D39E5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD8F09-88F3-4DCE-B882-4110EABF843C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="192">
   <si>
     <t>Name</t>
   </si>
@@ -509,9 +509,6 @@
   </si>
   <si>
     <t>Oversize Design</t>
-  </si>
-  <si>
-    <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/549 (Oversize).jpg</t>
   </si>
   <si>
     <t>Location Specific &gt; Sleeve</t>
@@ -1011,9 +1008,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAA5445-AEE9-4E73-8E71-AF32335F1380}">
   <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AE7" sqref="AE7"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AC8" sqref="AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,7 +1024,7 @@
     <col min="8" max="8" width="29.5703125" customWidth="1"/>
     <col min="9" max="9" width="19.85546875" customWidth="1"/>
     <col min="12" max="12" width="12.42578125" customWidth="1"/>
-    <col min="29" max="29" width="9.140625" style="1"/>
+    <col min="29" max="29" width="12" style="1" customWidth="1"/>
     <col min="31" max="31" width="71.140625" customWidth="1"/>
     <col min="32" max="32" width="71.85546875" customWidth="1"/>
     <col min="33" max="33" width="63.85546875" customWidth="1"/>
@@ -1054,13 +1051,13 @@
         <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G1" t="s">
+        <v>153</v>
+      </c>
+      <c r="H1" t="s">
         <v>154</v>
-      </c>
-      <c r="H1" t="s">
-        <v>155</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
@@ -1120,7 +1117,7 @@
         <v>135</v>
       </c>
       <c r="AB1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AC1" t="s">
         <v>136</v>
@@ -1129,7 +1126,7 @@
         <v>138</v>
       </c>
       <c r="AE1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AF1" t="s">
         <v>105</v>
@@ -1167,7 +1164,7 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -1188,13 +1185,13 @@
         <v>3</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD2" t="s">
         <v>140</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AF2" t="s">
         <v>37</v>
@@ -1214,13 +1211,13 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L3" t="s">
         <v>12</v>
@@ -1235,7 +1232,7 @@
         <v>30</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD3" t="s">
         <v>140</v>
@@ -1255,13 +1252,13 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
@@ -1270,13 +1267,13 @@
         <v>28</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD4" t="s">
         <v>140</v>
       </c>
       <c r="AF4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG4" t="s">
         <v>39</v>
@@ -1305,7 +1302,7 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -1326,7 +1323,7 @@
         <v>27</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD5" t="s">
         <v>140</v>
@@ -1346,13 +1343,13 @@
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L6" t="s">
         <v>12</v>
@@ -1364,7 +1361,7 @@
         <v>1</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD6" t="s">
         <v>140</v>
@@ -1384,13 +1381,13 @@
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L7" t="s">
         <v>12</v>
@@ -1399,7 +1396,7 @@
         <v>27</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD7" t="s">
         <v>140</v>
@@ -1419,13 +1416,13 @@
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L8" t="s">
         <v>12</v>
@@ -1434,7 +1431,7 @@
         <v>27</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD8" t="s">
         <v>140</v>
@@ -1454,13 +1451,13 @@
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L9" t="s">
         <v>12</v>
@@ -1469,7 +1466,7 @@
         <v>30</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD9" t="s">
         <v>140</v>
@@ -1489,13 +1486,13 @@
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L10" t="s">
         <v>12</v>
@@ -1507,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD10" t="s">
         <v>140</v>
@@ -1527,13 +1524,13 @@
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L11" t="s">
         <v>12</v>
@@ -1542,7 +1539,7 @@
         <v>31</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD11" t="s">
         <v>140</v>
@@ -1562,13 +1559,13 @@
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L12" t="s">
         <v>12</v>
@@ -1577,7 +1574,7 @@
         <v>27</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AD12" t="s">
         <v>140</v>
@@ -1594,7 +1591,7 @@
         <v>151</v>
       </c>
       <c r="D13" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -1603,19 +1600,19 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M13" t="s">
         <v>28</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AD13" t="s">
         <v>140</v>
       </c>
       <c r="AF13" t="s">
-        <v>152</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1651,9 +1648,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CAB92D6-74EB-48E1-B757-D6D5F24DBA22}">
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AD14" sqref="AD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1693,10 +1690,10 @@
         <v>49</v>
       </c>
       <c r="F1" t="s">
+        <v>153</v>
+      </c>
+      <c r="G1" t="s">
         <v>154</v>
-      </c>
-      <c r="G1" t="s">
-        <v>155</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1756,7 +1753,7 @@
         <v>135</v>
       </c>
       <c r="AA1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB1" t="s">
         <v>136</v>
@@ -1800,7 +1797,7 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -1815,7 +1812,7 @@
         <v>29</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AC2" t="s">
         <v>140</v>
@@ -1841,7 +1838,7 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -1865,7 +1862,7 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AC3" t="s">
         <v>140</v>
@@ -1885,7 +1882,7 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -1920,7 +1917,7 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
@@ -1938,7 +1935,7 @@
         <v>31</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AC5" t="s">
         <v>140</v>
@@ -1955,7 +1952,7 @@
         <v>142</v>
       </c>
       <c r="D6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -1976,7 +1973,7 @@
         <v>140</v>
       </c>
       <c r="AD6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -1987,7 +1984,7 @@
         <v>142</v>
       </c>
       <c r="D7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -2005,13 +2002,13 @@
         <v>2</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="AC7" t="s">
         <v>140</v>
       </c>
       <c r="AD7" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -2022,7 +2019,7 @@
         <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -2037,13 +2034,13 @@
         <v>29</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="AC8" t="s">
         <v>140</v>
       </c>
       <c r="AD8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -2054,7 +2051,7 @@
         <v>142</v>
       </c>
       <c r="D9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
@@ -2069,13 +2066,13 @@
         <v>29</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="AC9" t="s">
         <v>140</v>
       </c>
       <c r="AD9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -2086,7 +2083,7 @@
         <v>142</v>
       </c>
       <c r="D10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
@@ -2101,13 +2098,13 @@
         <v>29</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="AC10" t="s">
         <v>140</v>
       </c>
       <c r="AD10" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -2118,7 +2115,7 @@
         <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
@@ -2130,7 +2127,7 @@
         <v>29</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="AC11" t="s">
         <v>141</v>
@@ -2181,127 +2178,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bad filtering logic affecting embroidery designs; update tests and test data accordingly
</commit_message>
<xml_diff>
--- a/samples/sampleTempDb.xlsx
+++ b/samples/sampleTempDb.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.klope\Documents\Development\design-library-backend\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97DD8F09-88F3-4DCE-B882-4110EABF843C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656FE286-52F3-46DA-8FC0-BECE764364F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1755" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
+    <workbookView xWindow="-23148" yWindow="636" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{66E2A19B-EDCE-41E4-AEFB-3FE13F30B3A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Screen Print Designs" sheetId="7" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="188">
   <si>
     <t>Name</t>
   </si>
@@ -349,24 +349,12 @@
     <t>Holiday &gt; Veterans Day</t>
   </si>
   <si>
-    <t>Quick Search &gt; New Designs</t>
-  </si>
-  <si>
     <t>Location Specific &gt; Oversize</t>
   </si>
   <si>
-    <t>Union Specific &gt; International Logos</t>
-  </si>
-  <si>
     <t>Quick Search &gt; Staff Favorites</t>
   </si>
   <si>
-    <t>Union Specific &gt; NALC</t>
-  </si>
-  <si>
-    <t>Union Specific &gt; SEIU</t>
-  </si>
-  <si>
     <t>Design Number</t>
   </si>
   <si>
@@ -484,21 +472,6 @@
     <t>Union Swirl</t>
   </si>
   <si>
-    <t>Union Specific &gt; IAM</t>
-  </si>
-  <si>
-    <t>Union Specific &gt; IUEC</t>
-  </si>
-  <si>
-    <t>Union Specific &gt; Laborers</t>
-  </si>
-  <si>
-    <t>Union Specific &gt; UAW</t>
-  </si>
-  <si>
-    <t>Union Specific &gt; USW</t>
-  </si>
-  <si>
     <t>/Marketing/Website/Design Library/Downloaded Images 12-13-2023/205 (5).jpg</t>
   </si>
   <si>
@@ -629,6 +602,21 @@
   </si>
   <si>
     <t>https://www.imagepointe.com/wp-content/uploads/2024/02/1732-darks.png</t>
+  </si>
+  <si>
+    <t>International Union Logos &gt; APWU</t>
+  </si>
+  <si>
+    <t>Inspiration Board &gt; Chest/Sleeve</t>
+  </si>
+  <si>
+    <t>International Union Logos &gt; IATSE</t>
+  </si>
+  <si>
+    <t>International Union Logos &gt; NATCA</t>
+  </si>
+  <si>
+    <t>Inspiration Board &gt; Full Size Embroidery</t>
   </si>
 </sst>
 </file>
@@ -710,9 +698,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -750,7 +738,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -856,7 +844,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -998,7 +986,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1036,7 +1024,7 @@
   <sheetData>
     <row r="1" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1051,13 +1039,13 @@
         <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="G1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="H1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="I1" t="s">
         <v>9</v>
@@ -1087,70 +1075,70 @@
         <v>36</v>
       </c>
       <c r="R1" t="s">
+        <v>122</v>
+      </c>
+      <c r="S1" t="s">
+        <v>123</v>
+      </c>
+      <c r="T1" t="s">
+        <v>124</v>
+      </c>
+      <c r="U1" t="s">
+        <v>125</v>
+      </c>
+      <c r="V1" t="s">
         <v>126</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>127</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>128</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>129</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>130</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
         <v>131</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AB1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC1" t="s">
         <v>132</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AD1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL1" t="s">
         <v>133</v>
       </c>
-      <c r="Z1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AM1" t="s">
         <v>135</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>190</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.25">
@@ -1164,7 +1152,7 @@
         <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
@@ -1173,7 +1161,7 @@
         <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="L2" t="s">
         <v>12</v>
@@ -1185,13 +1173,13 @@
         <v>3</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AD2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AE2" s="3" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="AF2" t="s">
         <v>37</v>
@@ -1211,13 +1199,13 @@
         <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L3" t="s">
         <v>12</v>
@@ -1232,10 +1220,10 @@
         <v>30</v>
       </c>
       <c r="AC3" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF3" t="s">
         <v>40</v>
@@ -1252,13 +1240,13 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L4" t="s">
         <v>12</v>
@@ -1267,13 +1255,13 @@
         <v>28</v>
       </c>
       <c r="AC4" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF4" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="AG4" t="s">
         <v>39</v>
@@ -1302,16 +1290,16 @@
         <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
         <v>99</v>
-      </c>
-      <c r="H5" t="s">
-        <v>101</v>
       </c>
       <c r="L5" t="s">
         <v>12</v>
@@ -1323,10 +1311,10 @@
         <v>27</v>
       </c>
       <c r="AC5" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF5" t="s">
         <v>41</v>
@@ -1337,19 +1325,19 @@
         <v>1012</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
         <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L6" t="s">
         <v>12</v>
@@ -1361,10 +1349,10 @@
         <v>1</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AD6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF6" t="s">
         <v>41</v>
@@ -1375,19 +1363,19 @@
         <v>1013</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L7" t="s">
         <v>12</v>
@@ -1396,10 +1384,10 @@
         <v>27</v>
       </c>
       <c r="AC7" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF7" t="s">
         <v>40</v>
@@ -1410,19 +1398,19 @@
         <v>1014</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C8" t="s">
         <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E8" t="s">
         <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L8" t="s">
         <v>12</v>
@@ -1431,10 +1419,10 @@
         <v>27</v>
       </c>
       <c r="AC8" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AD8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF8" t="s">
         <v>40</v>
@@ -1445,19 +1433,19 @@
         <v>1015</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L9" t="s">
         <v>12</v>
@@ -1466,10 +1454,10 @@
         <v>30</v>
       </c>
       <c r="AC9" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF9" t="s">
         <v>43</v>
@@ -1480,19 +1468,19 @@
         <v>1016</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
         <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L10" t="s">
         <v>12</v>
@@ -1504,10 +1492,10 @@
         <v>2</v>
       </c>
       <c r="AC10" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF10" t="s">
         <v>41</v>
@@ -1518,19 +1506,19 @@
         <v>1017</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
         <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
         <v>14</v>
       </c>
       <c r="G11" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L11" t="s">
         <v>12</v>
@@ -1539,10 +1527,10 @@
         <v>31</v>
       </c>
       <c r="AC11" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD11" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF11" t="s">
         <v>43</v>
@@ -1553,19 +1541,19 @@
         <v>1018</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
         <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
         <v>14</v>
       </c>
       <c r="G12" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L12" t="s">
         <v>12</v>
@@ -1574,10 +1562,10 @@
         <v>27</v>
       </c>
       <c r="AC12" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AD12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF12" t="s">
         <v>40</v>
@@ -1588,10 +1576,10 @@
         <v>549</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D13" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
         <v>14</v>
@@ -1600,16 +1588,16 @@
         <v>1</v>
       </c>
       <c r="G13" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="M13" t="s">
         <v>28</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AD13" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AF13" t="s">
         <v>41</v>
@@ -1649,8 +1637,8 @@
   <dimension ref="A1:AK11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AB15" sqref="AB15"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1663,7 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1690,10 +1678,10 @@
         <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="G1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H1" t="s">
         <v>9</v>
@@ -1723,67 +1711,67 @@
         <v>36</v>
       </c>
       <c r="Q1" t="s">
+        <v>122</v>
+      </c>
+      <c r="R1" t="s">
+        <v>123</v>
+      </c>
+      <c r="S1" t="s">
+        <v>124</v>
+      </c>
+      <c r="T1" t="s">
+        <v>125</v>
+      </c>
+      <c r="U1" t="s">
         <v>126</v>
       </c>
-      <c r="R1" t="s">
+      <c r="V1" t="s">
         <v>127</v>
       </c>
-      <c r="S1" t="s">
+      <c r="W1" t="s">
         <v>128</v>
       </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
         <v>129</v>
       </c>
-      <c r="U1" t="s">
+      <c r="Y1" t="s">
         <v>130</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Z1" t="s">
         <v>131</v>
       </c>
-      <c r="W1" t="s">
+      <c r="AA1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AB1" t="s">
         <v>132</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AC1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>101</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>104</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>105</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ1" t="s">
         <v>133</v>
       </c>
-      <c r="Y1" t="s">
-        <v>134</v>
-      </c>
-      <c r="Z1" t="s">
+      <c r="AK1" t="s">
         <v>135</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>105</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>107</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>106</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>108</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>109</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.25">
@@ -1797,13 +1785,13 @@
         <v>24</v>
       </c>
       <c r="D2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
       </c>
       <c r="F2" t="s">
-        <v>112</v>
+        <v>183</v>
       </c>
       <c r="K2" t="s">
         <v>13</v>
@@ -1812,10 +1800,10 @@
         <v>29</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AC2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD2" t="s">
         <v>38</v>
@@ -1838,19 +1826,16 @@
         <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
+        <v>183</v>
       </c>
       <c r="G3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H3" t="s">
-        <v>103</v>
+        <v>187</v>
       </c>
       <c r="K3" t="s">
         <v>13</v>
@@ -1862,10 +1847,10 @@
         <v>1</v>
       </c>
       <c r="AB3" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AC3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD3" t="s">
         <v>39</v>
@@ -1882,13 +1867,13 @@
         <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
       <c r="F4" t="s">
-        <v>101</v>
+        <v>141</v>
       </c>
       <c r="K4" t="s">
         <v>13</v>
@@ -1897,7 +1882,7 @@
         <v>31</v>
       </c>
       <c r="AC4" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD4" t="s">
         <v>42</v>
@@ -1917,16 +1902,16 @@
         <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>100</v>
+        <v>183</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>184</v>
       </c>
       <c r="K5" t="s">
         <v>13</v>
@@ -1935,10 +1920,10 @@
         <v>31</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="AC5" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD5" t="s">
         <v>43</v>
@@ -1949,16 +1934,16 @@
         <v>205</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
@@ -1970,10 +1955,10 @@
         <v>3</v>
       </c>
       <c r="AC6" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD6" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:37" x14ac:dyDescent="0.25">
@@ -1981,16 +1966,16 @@
         <v>205</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>144</v>
+        <v>185</v>
       </c>
       <c r="K7" t="s">
         <v>13</v>
@@ -2002,13 +1987,13 @@
         <v>2</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AC7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD7" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:37" x14ac:dyDescent="0.25">
@@ -2016,16 +2001,16 @@
         <v>205</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>145</v>
+        <v>185</v>
       </c>
       <c r="K8" t="s">
         <v>13</v>
@@ -2034,13 +2019,13 @@
         <v>29</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AC8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
@@ -2048,16 +2033,16 @@
         <v>205</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>146</v>
+        <v>184</v>
       </c>
       <c r="K9" t="s">
         <v>13</v>
@@ -2066,13 +2051,13 @@
         <v>29</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AC9" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:37" x14ac:dyDescent="0.25">
@@ -2080,16 +2065,16 @@
         <v>205</v>
       </c>
       <c r="B10" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>147</v>
+        <v>186</v>
       </c>
       <c r="K10" t="s">
         <v>13</v>
@@ -2098,13 +2083,13 @@
         <v>29</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AC10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="AD10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:37" x14ac:dyDescent="0.25">
@@ -2112,28 +2097,28 @@
         <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="L11" t="s">
         <v>29</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="AC11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="AD11" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2142,7 +2127,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E11 E13:E1048576" xr:uid="{40D061BB-7D80-4843-BA97-3B750B8AB087}">
       <formula1>YesNo</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:J11 F13:J1048576" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F13:J1048576 F2:J11" xr:uid="{159C1945-644A-42BE-8D6B-9453D831D751}">
       <formula1>Subcategories</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L13:Z1048576 L2:Z11" xr:uid="{8CFC8C89-BCE5-409B-AB92-A66E5FAE516C}">
@@ -2178,127 +2163,127 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -2369,7 +2354,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
@@ -2377,7 +2362,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
@@ -3037,7 +3022,7 @@
         <v>65</v>
       </c>
       <c r="B53" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C53" t="str">
         <f t="shared" si="1"/>
@@ -3049,7 +3034,7 @@
         <v>66</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C54" t="str">
         <f t="shared" si="1"/>
@@ -3061,7 +3046,7 @@
         <v>67</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C55" t="str">
         <f t="shared" si="1"/>
@@ -3073,7 +3058,7 @@
         <v>68</v>
       </c>
       <c r="B56" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C56" t="str">
         <f t="shared" si="1"/>
@@ -3085,7 +3070,7 @@
         <v>69</v>
       </c>
       <c r="B57" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C57" t="str">
         <f t="shared" si="1"/>
@@ -3097,7 +3082,7 @@
         <v>70</v>
       </c>
       <c r="B58" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C58" t="str">
         <f t="shared" si="1"/>
@@ -3109,7 +3094,7 @@
         <v>71</v>
       </c>
       <c r="B59" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C59" t="str">
         <f t="shared" si="1"/>
@@ -3121,7 +3106,7 @@
         <v>72</v>
       </c>
       <c r="B60" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C60" t="str">
         <f t="shared" si="1"/>
@@ -3133,7 +3118,7 @@
         <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C61" t="str">
         <f t="shared" si="1"/>
@@ -3145,7 +3130,7 @@
         <v>74</v>
       </c>
       <c r="B62" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C62" t="str">
         <f t="shared" si="1"/>
@@ -3157,7 +3142,7 @@
         <v>75</v>
       </c>
       <c r="B63" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C63" t="str">
         <f t="shared" si="1"/>
@@ -3169,7 +3154,7 @@
         <v>76</v>
       </c>
       <c r="B64" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C64" t="str">
         <f t="shared" si="1"/>
@@ -3181,7 +3166,7 @@
         <v>77</v>
       </c>
       <c r="B65" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C65" t="str">
         <f t="shared" si="1"/>
@@ -3193,7 +3178,7 @@
         <v>17</v>
       </c>
       <c r="B66" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C66" t="str">
         <f t="shared" si="1"/>
@@ -3205,7 +3190,7 @@
         <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C67" t="str">
         <f t="shared" si="1"/>
@@ -3217,7 +3202,7 @@
         <v>79</v>
       </c>
       <c r="B68" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C68" t="str">
         <f t="shared" si="1"/>
@@ -3229,7 +3214,7 @@
         <v>80</v>
       </c>
       <c r="B69" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C69" t="str">
         <f t="shared" si="1"/>
@@ -3241,7 +3226,7 @@
         <v>81</v>
       </c>
       <c r="B70" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C70" t="str">
         <f t="shared" si="1"/>
@@ -3253,7 +3238,7 @@
         <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="1"/>
@@ -3265,7 +3250,7 @@
         <v>83</v>
       </c>
       <c r="B72" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C72" t="str">
         <f t="shared" si="1"/>
@@ -3277,7 +3262,7 @@
         <v>84</v>
       </c>
       <c r="B73" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C73" t="str">
         <f t="shared" si="1"/>
@@ -3289,7 +3274,7 @@
         <v>85</v>
       </c>
       <c r="B74" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C74" t="str">
         <f t="shared" si="1"/>
@@ -3301,7 +3286,7 @@
         <v>86</v>
       </c>
       <c r="B75" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C75" t="str">
         <f t="shared" si="1"/>
@@ -3313,7 +3298,7 @@
         <v>87</v>
       </c>
       <c r="B76" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C76" t="str">
         <f t="shared" si="1"/>
@@ -3325,7 +3310,7 @@
         <v>16</v>
       </c>
       <c r="B77" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C77" t="str">
         <f t="shared" si="1"/>
@@ -3337,7 +3322,7 @@
         <v>88</v>
       </c>
       <c r="B78" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C78" t="str">
         <f t="shared" si="1"/>
@@ -3349,7 +3334,7 @@
         <v>89</v>
       </c>
       <c r="B79" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="1"/>
@@ -3361,7 +3346,7 @@
         <v>90</v>
       </c>
       <c r="B80" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="1"/>
@@ -3373,7 +3358,7 @@
         <v>91</v>
       </c>
       <c r="B81" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C81" t="str">
         <f t="shared" si="1"/>
@@ -3385,7 +3370,7 @@
         <v>92</v>
       </c>
       <c r="B82" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C82" t="str">
         <f t="shared" si="1"/>
@@ -3397,7 +3382,7 @@
         <v>93</v>
       </c>
       <c r="B83" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C83" t="str">
         <f t="shared" si="1"/>
@@ -3406,10 +3391,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B84" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C84" t="str">
         <f t="shared" si="1"/>
@@ -3418,10 +3403,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B85" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C85" t="str">
         <f t="shared" si="1"/>
@@ -3430,10 +3415,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B86" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C86" t="str">
         <f t="shared" si="1"/>
@@ -3442,10 +3427,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B87" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C87" t="str">
         <f t="shared" si="1"/>
@@ -3474,17 +3459,17 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3514,7 +3499,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>
@@ -3589,7 +3574,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>